<commit_message>
updated component list (changes made by Raffael)
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="225"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="225"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="180">
   <si>
     <t>CPIO - Cuisine Purpose Input/Output Board</t>
   </si>
@@ -190,6 +190,21 @@
   </si>
   <si>
     <t>0.1u</t>
+  </si>
+  <si>
+    <t>Status LED</t>
+  </si>
+  <si>
+    <t>green, V_R=12V (knapp). What is V_R?</t>
+  </si>
+  <si>
+    <t>“0805”</t>
+  </si>
+  <si>
+    <t>475-1410-1-ND</t>
+  </si>
+  <si>
+    <t>$0.21</t>
   </si>
   <si>
     <t>R_led_12V</t>
@@ -662,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -697,6 +712,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1159,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1472,11 +1490,20 @@
       <c r="A20" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="1">
-        <v>490</v>
+      <c r="B20" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="D20">
         <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>27</v>
@@ -1484,93 +1511,93 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="B21" s="1">
+        <v>490</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="G21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>57</v>
+      <c r="I21" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>60</v>
-      </c>
-      <c r="I24" t="s">
-        <v>35</v>
+      <c r="A24" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>62</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>65</v>
+      <c r="A28" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="I29" s="11" t="s">
-        <v>27</v>
+      <c r="E29" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1581,7 +1608,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1592,10 +1622,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1606,10 +1633,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1620,10 +1647,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1634,13 +1661,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="D35">
         <v>1</v>
-      </c>
-      <c r="G35" t="s">
-        <v>78</v>
       </c>
       <c r="I35" s="11" t="s">
         <v>27</v>
@@ -1648,251 +1675,250 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="E36" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F36" s="18">
+      <c r="G36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" s="19">
         <v>0.311</v>
       </c>
-      <c r="I36" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="19">
-        <v>1</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F37" s="19" t="s">
+      <c r="I37" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G37" s="19" t="s">
+    </row>
+    <row r="38" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="I37" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
+      <c r="B38" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="I38" s="22"/>
-    </row>
-    <row r="39" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="C38" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="D38" s="20">
+        <v>1</v>
+      </c>
+      <c r="E38" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="F38" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="18" t="s">
+      <c r="G38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="F39" s="18">
+      <c r="I38" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="I39" s="23"/>
+    </row>
+    <row r="40" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" s="19">
         <v>0.34800000000000003</v>
       </c>
-      <c r="G39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>96</v>
+      <c r="G40" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D42" s="26">
+      <c r="A42" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="27">
         <v>4</v>
       </c>
-      <c r="E42" t="s">
-        <v>99</v>
-      </c>
-      <c r="G42" t="s">
-        <v>100</v>
-      </c>
-      <c r="H42" t="s">
-        <v>101</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="25"/>
-      <c r="B43" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="26">
-        <v>4</v>
-      </c>
       <c r="E43" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H43" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="I43" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="26"/>
+      <c r="B44" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="D44" s="27">
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" t="s">
+        <v>108</v>
+      </c>
+      <c r="H44" t="s">
+        <v>106</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="28">
         <v>6</v>
       </c>
-      <c r="I44" s="27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D45" s="11">
-        <v>1</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F45" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="I45" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D46">
-        <v>4</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="C46" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="I46" s="11" t="s">
-        <v>19</v>
+      <c r="D46" s="11">
+        <v>1</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>113</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>116</v>
       </c>
       <c r="D47">
         <v>4</v>
       </c>
+      <c r="E47" t="s">
+        <v>117</v>
+      </c>
       <c r="I47" s="11" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>115</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C48" s="30"/>
+        <v>118</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>119</v>
+      </c>
       <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="F48" s="11"/>
+        <v>4</v>
+      </c>
       <c r="I48" s="11" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="26">
+      <c r="A49" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="31"/>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="11"/>
+      <c r="I49" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="27">
         <v>2</v>
       </c>
-      <c r="E49" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="G49" t="s">
-        <v>120</v>
-      </c>
-      <c r="H49" t="s">
-        <v>121</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>122</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" s="13"/>
-      <c r="D50">
-        <v>2</v>
+      <c r="E50" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="G50" t="s">
+        <v>125</v>
+      </c>
+      <c r="H50" t="s">
+        <v>126</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>19</v>
@@ -1900,231 +1926,232 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>124</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>125</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="13"/>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>126</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>130</v>
       </c>
       <c r="D52">
         <v>2</v>
       </c>
-      <c r="F52" s="26"/>
       <c r="I52" s="11" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="13"/>
+      <c r="A53" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="D53">
         <v>2</v>
       </c>
-      <c r="E53" t="s">
-        <v>130</v>
-      </c>
+      <c r="F53" s="27"/>
       <c r="I53" s="11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>131</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>132</v>
+      <c r="A54" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54">
         <v>2</v>
       </c>
+      <c r="E54" t="s">
+        <v>135</v>
+      </c>
       <c r="I54" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>134</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B55" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="13"/>
       <c r="D55">
         <v>2</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>135</v>
-      </c>
-      <c r="B56" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>139</v>
+      </c>
       <c r="D56">
         <v>2</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="B57" s="31"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="26" t="s">
-        <v>83</v>
+      <c r="A57" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="D57">
+        <v>2</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>137</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="A58" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" s="32"/>
       <c r="C58" s="13"/>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>139</v>
-      </c>
-      <c r="G58" t="s">
-        <v>49</v>
-      </c>
-      <c r="H58" t="s">
-        <v>121</v>
+      <c r="D58" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="C59" s="13"/>
       <c r="D59">
         <v>1</v>
       </c>
+      <c r="E59" t="s">
+        <v>144</v>
+      </c>
+      <c r="G59" t="s">
+        <v>49</v>
+      </c>
+      <c r="H59" t="s">
+        <v>126</v>
+      </c>
       <c r="I59" s="11" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>142</v>
-      </c>
-      <c r="B60" s="29" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
-      <c r="G60" t="s">
-        <v>144</v>
-      </c>
-      <c r="H60" t="s">
-        <v>145</v>
-      </c>
       <c r="I60" s="11" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>146</v>
-      </c>
-      <c r="B61" s="2"/>
+        <v>147</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>148</v>
+      </c>
       <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="G61" t="s">
+        <v>149</v>
+      </c>
+      <c r="H61" t="s">
+        <v>150</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>151</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="D62">
         <v>4</v>
       </c>
-      <c r="F61" t="s">
-        <v>147</v>
-      </c>
-      <c r="I61" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C63" s="13"/>
+      <c r="F62" t="s">
+        <v>152</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>149</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D64">
+      <c r="A64" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" s="13"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65">
         <f>4+2+1+1+6</f>
         <v>14</v>
       </c>
-      <c r="E64" t="s">
-        <v>151</v>
-      </c>
-      <c r="G64" t="s">
-        <v>152</v>
-      </c>
-      <c r="H64" t="s">
-        <v>153</v>
-      </c>
-      <c r="I64" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>53</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D65">
-        <v>14</v>
-      </c>
-      <c r="I65" s="11" t="s">
-        <v>27</v>
+      <c r="E65" t="s">
+        <v>156</v>
+      </c>
+      <c r="G65" t="s">
+        <v>157</v>
+      </c>
+      <c r="H65" t="s">
+        <v>158</v>
+      </c>
+      <c r="I65" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>156</v>
-      </c>
-      <c r="B66" s="29" t="s">
-        <v>157</v>
+        <v>53</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I66" s="11" t="s">
         <v>27</v>
@@ -2132,9 +2159,11 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>158</v>
-      </c>
-      <c r="B67" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="B67" s="30" t="s">
+        <v>162</v>
+      </c>
       <c r="D67">
         <v>3</v>
       </c>
@@ -2144,16 +2173,11 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>159</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>160</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="B68" s="2"/>
       <c r="D68">
-        <v>1</v>
-      </c>
-      <c r="E68" t="s">
-        <v>161</v>
+        <v>3</v>
       </c>
       <c r="I68" s="11" t="s">
         <v>27</v>
@@ -2161,14 +2185,16 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C69" s="13"/>
+        <v>165</v>
+      </c>
       <c r="D69">
         <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>166</v>
       </c>
       <c r="I69" s="11" t="s">
         <v>27</v>
@@ -2176,16 +2202,14 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="C70" s="13"/>
       <c r="D70">
         <v>1</v>
-      </c>
-      <c r="E70" t="s">
-        <v>165</v>
       </c>
       <c r="I70" s="11" t="s">
         <v>27</v>
@@ -2193,40 +2217,45 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>127</v>
+        <v>18</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
+      <c r="E71" t="s">
+        <v>170</v>
+      </c>
       <c r="I71" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="8" t="s">
-        <v>167</v>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>171</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="I72" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>168</v>
-      </c>
-      <c r="B74" s="31"/>
-      <c r="D74">
-        <v>4</v>
-      </c>
-      <c r="I74" s="11" t="s">
-        <v>19</v>
+      <c r="A74" s="8" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>169</v>
-      </c>
-      <c r="B75" s="31"/>
+        <v>173</v>
+      </c>
+      <c r="B75" s="32"/>
       <c r="D75">
         <v>4</v>
       </c>
@@ -2236,33 +2265,33 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>170</v>
-      </c>
-      <c r="B76" s="31"/>
+        <v>174</v>
+      </c>
+      <c r="B76" s="32"/>
       <c r="D76">
         <v>4</v>
       </c>
       <c r="I76" s="11" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>171</v>
-      </c>
-      <c r="B77" s="31"/>
+        <v>175</v>
+      </c>
+      <c r="B77" s="32"/>
       <c r="D77">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>172</v>
-      </c>
-      <c r="B78" s="31"/>
+        <v>176</v>
+      </c>
+      <c r="B78" s="32"/>
       <c r="D78">
         <v>1</v>
       </c>
@@ -2272,37 +2301,49 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>173</v>
-      </c>
-      <c r="B79" s="31"/>
+        <v>177</v>
+      </c>
+      <c r="B79" s="32"/>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>174</v>
-      </c>
-      <c r="B80" s="31"/>
-      <c r="D80" s="26" t="s">
-        <v>83</v>
+        <v>178</v>
+      </c>
+      <c r="B80" s="32"/>
+      <c r="D80">
+        <v>1</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>179</v>
+      </c>
+      <c r="B81" s="32"/>
+      <c r="D81" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="I81" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="B36" r:id="rId1"/>
-    <hyperlink ref="E36" r:id="rId2"/>
-    <hyperlink ref="B37" r:id="rId3"/>
-    <hyperlink ref="E37" r:id="rId4"/>
-    <hyperlink ref="E39" r:id="rId5"/>
-    <hyperlink ref="E45" r:id="rId6"/>
+    <hyperlink ref="B37" r:id="rId1"/>
+    <hyperlink ref="E37" r:id="rId2"/>
+    <hyperlink ref="B38" r:id="rId3"/>
+    <hyperlink ref="E38" r:id="rId4"/>
+    <hyperlink ref="E40" r:id="rId5"/>
+    <hyperlink ref="E46" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
clean start with components population of Eagle library
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="225"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="225"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="178">
   <si>
     <t>CPIO - Cuisine Purpose Input/Output Board</t>
   </si>
@@ -60,9 +60,6 @@
     <t>RP Pin</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>S2012EC-20-ND</t>
   </si>
   <si>
-    <t>Sparkfun</t>
-  </si>
-  <si>
     <t>40 Pin Header, female</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>1528-1385-ND</t>
   </si>
   <si>
-    <t>Required? Available Space?</t>
-  </si>
-  <si>
     <t>Spacer</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t>AE10793-ND</t>
   </si>
   <si>
-    <t>to do</t>
-  </si>
-  <si>
     <t>Power Input</t>
   </si>
   <si>
@@ -156,15 +144,9 @@
     <t>Switch</t>
   </si>
   <si>
-    <t>28V, 5A</t>
-  </si>
-  <si>
     <t>EG5137-ND</t>
   </si>
   <si>
-    <t>To switch what?</t>
-  </si>
-  <si>
     <t>Power Measurement IC</t>
   </si>
   <si>
@@ -177,9 +159,6 @@
     <t>via I2C</t>
   </si>
   <si>
-    <t>UL</t>
-  </si>
-  <si>
     <t>R_sense</t>
   </si>
   <si>
@@ -195,18 +174,9 @@
     <t>Status LED</t>
   </si>
   <si>
-    <t>green, V_R=12V (knapp). What is V_R?</t>
-  </si>
-  <si>
-    <t>“0805”</t>
-  </si>
-  <si>
     <t>475-1410-1-ND</t>
   </si>
   <si>
-    <t>$0.21</t>
-  </si>
-  <si>
     <t>R_led_12V</t>
   </si>
   <si>
@@ -504,9 +474,6 @@
     <t>GPIO 18</t>
   </si>
   <si>
-    <t>Adafruit</t>
-  </si>
-  <si>
     <t>104???</t>
   </si>
   <si>
@@ -565,6 +532,33 @@
   </si>
   <si>
     <t>Garden Lightning</t>
+  </si>
+  <si>
+    <t>M20x2</t>
+  </si>
+  <si>
+    <t>indiv.</t>
+  </si>
+  <si>
+    <t>500SSP1S2M2, 28V, 5A</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>TSSOP-14</t>
+  </si>
+  <si>
+    <t>R_aux_up</t>
+  </si>
+  <si>
+    <t>R_aux_dn</t>
+  </si>
+  <si>
+    <t>2.75mm (diameter)</t>
   </si>
 </sst>
 </file>
@@ -574,7 +568,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -620,8 +614,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -648,12 +649,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="29"/>
-        <bgColor indexed="45"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="43"/>
         <bgColor indexed="13"/>
       </patternFill>
@@ -674,10 +669,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -711,23 +709,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -743,8 +737,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1177,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1194,12 +1199,12 @@
     <col min="7" max="7" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1215,13 +1220,13 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:13" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1246,1104 +1251,981 @@
       <c r="H4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
-      <c r="L5" s="14" t="s">
+      <c r="K5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="11" t="s">
+    </row>
+    <row r="6" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
-      <c r="L6" s="15" t="s">
+      <c r="K6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="11" t="s">
+    </row>
+    <row r="7" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="C7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="11">
-        <v>1</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="K7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="L7" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="11">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="11" t="s">
+    </row>
+    <row r="9" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="C9" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="11">
-        <v>1</v>
-      </c>
-      <c r="E9" s="11" t="s">
+    </row>
+    <row r="10" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="C10" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="11">
-        <v>1</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="13" t="s">
+        <v>177</v>
+      </c>
       <c r="D11" s="11">
         <v>2</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="G11" s="31"/>
+    </row>
+    <row r="12" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G12" s="31"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="32"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C15" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="11" t="s">
+      <c r="F15" s="11"/>
+      <c r="G15" s="32"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="I14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="G16" s="31"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="B17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="I15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="G17" t="s">
         <v>43</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="B18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C18" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C19" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>48</v>
       </c>
-      <c r="G17" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>49</v>
       </c>
-      <c r="I17" t="s">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>60</v>
       </c>
       <c r="B21" s="1">
         <v>490</v>
       </c>
+      <c r="C21" s="33" t="s">
+        <v>172</v>
+      </c>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="1">
+        <v>490</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>61</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="B32" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
-      <c r="I25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
+      <c r="B35" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>72</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="1" t="s">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>74</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B39" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C39" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="F39" s="17">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B40" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C40" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="D40" s="18">
+        <v>1</v>
+      </c>
+      <c r="E40" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="F40" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="I36" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="G40" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="19" t="s">
+    </row>
+    <row r="41" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+    </row>
+    <row r="42" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>86</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="19" t="s">
+      <c r="B42" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="19">
-        <v>0.311</v>
-      </c>
-      <c r="I37" s="11" t="s">
+      <c r="C42" s="17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="20" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="F42" s="17">
+        <v>0.34800000000000003</v>
+      </c>
+      <c r="G42" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="21" t="s">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D38" s="20">
-        <v>1</v>
-      </c>
-      <c r="E38" s="21" t="s">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="B45" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="D45" s="25">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
         <v>94</v>
       </c>
-      <c r="I38" s="20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="23" t="s">
+      <c r="G45" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="I39" s="23"/>
-    </row>
-    <row r="40" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="H45" t="s">
         <v>96</v>
       </c>
-      <c r="B40" s="19" t="s">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="24"/>
+      <c r="B46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="25">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="G46" t="s">
         <v>98</v>
       </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" s="19" t="s">
+      <c r="H46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="F40" s="19">
-        <v>0.34800000000000003</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
+      <c r="B48" s="17" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="D48" s="11">
+        <v>1</v>
+      </c>
+      <c r="E48" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D43" s="27">
+      <c r="F48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49">
         <v>4</v>
       </c>
-      <c r="E43" t="s">
-        <v>104</v>
-      </c>
-      <c r="G43" t="s">
-        <v>105</v>
-      </c>
-      <c r="H43" t="s">
-        <v>106</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="26"/>
-      <c r="B44" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="27">
+      <c r="E49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50">
         <v>4</v>
       </c>
-      <c r="E44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" t="s">
-        <v>108</v>
-      </c>
-      <c r="H44" t="s">
-        <v>106</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="28">
-        <v>6</v>
-      </c>
-      <c r="I45" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B51" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C51" s="29"/>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="11"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="11">
-        <v>1</v>
-      </c>
-      <c r="E46" s="19" t="s">
+      <c r="B52" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F46" t="s">
+      <c r="C52" s="13"/>
+      <c r="D52" s="25">
+        <v>2</v>
+      </c>
+      <c r="E52" s="25" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="G52" t="s">
         <v>115</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="H52" t="s">
         <v>116</v>
       </c>
-      <c r="D47">
-        <v>4</v>
-      </c>
-      <c r="E47" t="s">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>117</v>
       </c>
-      <c r="I47" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="B53" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="D48">
-        <v>4</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>120</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C49" s="31"/>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="F49" s="11"/>
-      <c r="I49" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="27">
-        <v>2</v>
-      </c>
-      <c r="E50" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="G50" t="s">
-        <v>125</v>
-      </c>
-      <c r="H50" t="s">
-        <v>126</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>127</v>
-      </c>
-      <c r="B51" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="C51" s="13"/>
-      <c r="D51">
-        <v>2</v>
-      </c>
-      <c r="I51" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>129</v>
-      </c>
-      <c r="B52" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52">
-        <v>2</v>
-      </c>
-      <c r="I52" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>131</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="C53" s="13"/>
       <c r="D53">
         <v>2</v>
       </c>
-      <c r="F53" s="27"/>
-      <c r="I53" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C54" s="13"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>120</v>
+      </c>
       <c r="D54">
         <v>2</v>
       </c>
-      <c r="E54" t="s">
-        <v>135</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>136</v>
-      </c>
-      <c r="B55" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C55" s="13"/>
+        <v>121</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="D55">
         <v>2</v>
       </c>
-      <c r="I55" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>138</v>
-      </c>
-      <c r="B56" s="30" t="s">
-        <v>139</v>
-      </c>
+      <c r="F55" s="25"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="13"/>
       <c r="D56">
         <v>2</v>
       </c>
-      <c r="I56" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>140</v>
-      </c>
-      <c r="B57" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="B57" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" s="13"/>
       <c r="D57">
         <v>2</v>
       </c>
-      <c r="I57" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="26" t="s">
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="D59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" s="30"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>132</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>134</v>
+      </c>
+      <c r="G61" t="s">
+        <v>43</v>
+      </c>
+      <c r="H61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>135</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>137</v>
+      </c>
+      <c r="B63" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>139</v>
+      </c>
+      <c r="H63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>141</v>
       </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B64" s="2"/>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="F64" t="s">
         <v>142</v>
       </c>
-      <c r="B59" s="1" t="s">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C59" s="13"/>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="C66" s="13"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>144</v>
       </c>
-      <c r="G59" t="s">
-        <v>49</v>
-      </c>
-      <c r="H59" t="s">
-        <v>126</v>
-      </c>
-      <c r="I59" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B67" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="I60" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>147</v>
-      </c>
-      <c r="B61" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="G61" t="s">
-        <v>149</v>
-      </c>
-      <c r="H61" t="s">
-        <v>150</v>
-      </c>
-      <c r="I61" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>151</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="D62">
-        <v>4</v>
-      </c>
-      <c r="F62" t="s">
-        <v>152</v>
-      </c>
-      <c r="I62" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C64" s="13"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>154</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D65">
+      <c r="D67">
         <f>4+2+1+1+6</f>
         <v>14</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E67" t="s">
+        <v>146</v>
+      </c>
+      <c r="G67" t="s">
+        <v>147</v>
+      </c>
+      <c r="H67" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D68">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>150</v>
+      </c>
+      <c r="B69" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>152</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="D70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>153</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>156</v>
       </c>
-      <c r="G65" t="s">
+      <c r="B72" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H65" t="s">
+      <c r="C72" s="13"/>
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>158</v>
       </c>
-      <c r="I65" t="s">
+      <c r="B73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" s="2" t="s">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>160</v>
       </c>
-      <c r="D66">
-        <v>14</v>
-      </c>
-      <c r="I66" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B74" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B67" s="30" t="s">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>162</v>
       </c>
-      <c r="D67">
-        <v>3</v>
-      </c>
-      <c r="I67" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>163</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="D68">
-        <v>3</v>
-      </c>
-      <c r="I68" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>164</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-      <c r="E69" t="s">
-        <v>166</v>
-      </c>
-      <c r="I69" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>167</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C70" s="13"/>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="I70" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>169</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="E71" t="s">
-        <v>170</v>
-      </c>
-      <c r="I71" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>171</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>173</v>
-      </c>
-      <c r="B75" s="32"/>
-      <c r="D75">
-        <v>4</v>
-      </c>
-      <c r="I75" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>174</v>
-      </c>
-      <c r="B76" s="32"/>
-      <c r="D76">
-        <v>4</v>
-      </c>
-      <c r="I76" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>175</v>
-      </c>
-      <c r="B77" s="32"/>
+      <c r="B77" s="30"/>
       <c r="D77">
         <v>4</v>
       </c>
-      <c r="I77" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>176</v>
-      </c>
-      <c r="B78" s="32"/>
+        <v>163</v>
+      </c>
+      <c r="B78" s="30"/>
       <c r="D78">
-        <v>1</v>
-      </c>
-      <c r="I78" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>177</v>
-      </c>
-      <c r="B79" s="32"/>
+        <v>164</v>
+      </c>
+      <c r="B79" s="30"/>
       <c r="D79">
-        <v>1</v>
-      </c>
-      <c r="I79" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>178</v>
-      </c>
-      <c r="B80" s="32"/>
+        <v>165</v>
+      </c>
+      <c r="B80" s="30"/>
       <c r="D80">
         <v>1</v>
       </c>
-      <c r="I80" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>179</v>
-      </c>
-      <c r="B81" s="32"/>
-      <c r="D81" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I81" s="11" t="s">
-        <v>88</v>
+        <v>166</v>
+      </c>
+      <c r="B81" s="30"/>
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" s="30"/>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>168</v>
+      </c>
+      <c r="B83" s="30"/>
+      <c r="D83" s="25" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="B37" r:id="rId1"/>
-    <hyperlink ref="E37" r:id="rId2"/>
-    <hyperlink ref="B38" r:id="rId3"/>
-    <hyperlink ref="E38" r:id="rId4"/>
-    <hyperlink ref="E40" r:id="rId5"/>
-    <hyperlink ref="E46" r:id="rId6"/>
+    <hyperlink ref="B39" r:id="rId1"/>
+    <hyperlink ref="E39" r:id="rId2"/>
+    <hyperlink ref="B40" r:id="rId3"/>
+    <hyperlink ref="E40" r:id="rId4"/>
+    <hyperlink ref="E42" r:id="rId5"/>
+    <hyperlink ref="E48" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
updated footprints and cleaned component list
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="183">
   <si>
     <t>CPIO - Cuisine Purpose Input/Output Board</t>
   </si>
@@ -192,9 +192,6 @@
     <t>VNQ5E160K-E</t>
   </si>
   <si>
-    <t>VNQ5E160K-E-ND</t>
-  </si>
-  <si>
     <t>...</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>LED LDO (5 to 4V)</t>
-  </si>
-  <si>
     <t>MIC5209-4.2YS, 4.2V, 500mA</t>
   </si>
   <si>
@@ -276,15 +270,9 @@
     <t>576-2372-ND</t>
   </si>
   <si>
-    <t>$1.19</t>
-  </si>
-  <si>
     <t>Quite big and expensive  due to high current and exotic voltage. All LEDs on could draw more max current</t>
   </si>
   <si>
-    <t>Level Shifter for 3.3 to 5V for LED command instead of additional LDO for LEDs. Drive LEDs with 5V</t>
-  </si>
-  <si>
     <t>LDO Sensor &amp; ADC (5 to 3.3?V)</t>
   </si>
   <si>
@@ -339,18 +327,12 @@
     <t>568-5262-1-ND</t>
   </si>
   <si>
-    <t>$0.51</t>
-  </si>
-  <si>
     <t>1-Wire Plug</t>
   </si>
   <si>
     <t>3x, JST with cable</t>
   </si>
   <si>
-    <t>Conrad &amp; Adafruit</t>
-  </si>
-  <si>
     <t>1-Wire Socket</t>
   </si>
   <si>
@@ -453,9 +435,6 @@
     <t>R_spi</t>
   </si>
   <si>
-    <t>$5.02</t>
-  </si>
-  <si>
     <t>Sensor Control</t>
   </si>
   <si>
@@ -480,9 +459,6 @@
     <t>Random Status LED</t>
   </si>
   <si>
-    <t>different colors? Same as for Power: simple BOM!</t>
-  </si>
-  <si>
     <t>R_led_3.3V</t>
   </si>
   <si>
@@ -559,6 +535,45 @@
   </si>
   <si>
     <t>2.75mm (diameter)</t>
+  </si>
+  <si>
+    <t>R_prot</t>
+  </si>
+  <si>
+    <t>R_gnd</t>
+  </si>
+  <si>
+    <t>Diode_gnd</t>
+  </si>
+  <si>
+    <t>PowerSSO-24</t>
+  </si>
+  <si>
+    <t>SOT23-6</t>
+  </si>
+  <si>
+    <t>497-11721-1-ND</t>
+  </si>
+  <si>
+    <t>Level Shifter (5 to 3.3V) for LED command instead of additional LDO for LEDs. Drive LEDs with 5V</t>
+  </si>
+  <si>
+    <t>LDO LED  (5 to 4V)</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Footprint missing</t>
+  </si>
+  <si>
+    <t>[Conrad / Adafruit]</t>
+  </si>
+  <si>
+    <t>10-TFSOP</t>
+  </si>
+  <si>
+    <t>indv.</t>
   </si>
 </sst>
 </file>
@@ -622,7 +637,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,14 +664,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="13"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-        <bgColor indexed="49"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="60"/>
       </patternFill>
     </fill>
   </fills>
@@ -669,13 +696,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -706,22 +744,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -729,12 +754,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -745,11 +764,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1182,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1194,8 +1263,8 @@
     <col min="2" max="2" width="30" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="24" customWidth="1"/>
     <col min="7" max="7" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1218,13 +1287,13 @@
       <c r="E2" s="7">
         <v>42338</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="25"/>
     </row>
     <row r="4" spans="1:12" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -1242,7 +1311,7 @@
       <c r="E4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="26" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -1255,10 +1324,11 @@
     <row r="5" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
-      <c r="K5" s="14" t="s">
+      <c r="F5" s="27"/>
+      <c r="K5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="34" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1268,10 +1338,11 @@
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
-      <c r="K6" s="15" t="s">
+      <c r="F6" s="27"/>
+      <c r="K6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="34" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1291,10 +1362,11 @@
       <c r="E7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="F7" s="27"/>
+      <c r="K7" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="34" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1314,8 +1386,15 @@
       <c r="E8" s="11" t="s">
         <v>18</v>
       </c>
+      <c r="F8" s="27"/>
       <c r="G8" s="11" t="s">
         <v>22</v>
+      </c>
+      <c r="K8" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1326,13 +1405,16 @@
         <v>24</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>25</v>
+      </c>
+      <c r="F9" s="27">
+        <v>0.63700000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1343,7 +1425,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
@@ -1351,7 +1433,10 @@
       <c r="E10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="31"/>
+      <c r="F10" s="27">
+        <v>2.25</v>
+      </c>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
@@ -1361,7 +1446,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D11" s="11">
         <v>2</v>
@@ -1369,18 +1454,22 @@
       <c r="E11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="31"/>
+      <c r="F11" s="27">
+        <v>0.34</v>
+      </c>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
-      <c r="G12" s="31"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1396,8 +1485,8 @@
       <c r="E14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="32"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1407,7 +1496,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1415,18 +1504,20 @@
       <c r="E15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="32"/>
+      <c r="F15" s="27">
+        <v>0.752</v>
+      </c>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1434,7 +1525,10 @@
       <c r="E16" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="31"/>
+      <c r="F16" s="24">
+        <v>2.609</v>
+      </c>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1444,13 +1538,16 @@
         <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>42</v>
+      </c>
+      <c r="F17" s="24">
+        <v>5.4335399999999998</v>
       </c>
       <c r="G17" t="s">
         <v>43</v>
@@ -1463,8 +1560,8 @@
       <c r="B18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="33" t="s">
-        <v>172</v>
+      <c r="C18" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1477,8 +1574,8 @@
       <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="33" t="s">
-        <v>172</v>
+      <c r="C19" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1489,14 +1586,17 @@
         <v>48</v>
       </c>
       <c r="B20" s="13"/>
-      <c r="C20" s="34" t="s">
-        <v>172</v>
+      <c r="C20" s="23" t="s">
+        <v>164</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>49</v>
+      </c>
+      <c r="F20" s="24">
+        <v>0.20699999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1506,8 +1606,8 @@
       <c r="B21" s="1">
         <v>490</v>
       </c>
-      <c r="C21" s="33" t="s">
-        <v>172</v>
+      <c r="C21" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1515,13 +1615,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>172</v>
+        <v>149</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1529,13 +1629,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B23" s="1">
         <v>490</v>
       </c>
-      <c r="C23" s="33" t="s">
-        <v>172</v>
+      <c r="C23" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1543,7 +1643,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1564,71 +1664,92 @@
       <c r="B27" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C27" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>175</v>
+      </c>
+      <c r="F27" s="24">
+        <v>3.504</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="D33">
         <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="24">
+        <v>0.7</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1636,10 +1757,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1647,10 +1771,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1658,10 +1782,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1669,565 +1796,720 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>67</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D38">
         <v>1</v>
-      </c>
-      <c r="G38" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="C41" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
         <v>76</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="F39" s="17">
+      <c r="F41" s="28">
         <v>0.311</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
+    <row r="42" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B42" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="D42" s="20">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="F42" s="32">
+        <v>1.19</v>
+      </c>
+      <c r="G42" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D40" s="18">
-        <v>1</v>
-      </c>
-      <c r="E40" s="19" t="s">
+    </row>
+    <row r="43" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>82</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="B44" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="18" t="s">
+      <c r="C44" s="38" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="21" t="s">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-    </row>
-    <row r="42" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="F44" s="28">
+        <v>0.34800000000000003</v>
+      </c>
+      <c r="G44" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="17" t="s">
+    </row>
+    <row r="45" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="17" t="s">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" s="17" t="s">
+      <c r="B47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F42" s="17">
-        <v>0.34800000000000003</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="C47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="16">
+        <v>4</v>
+      </c>
+      <c r="E47" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
+      <c r="F47" s="24">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="G47" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="24" t="s">
+      <c r="H47" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="1" t="s">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="15"/>
+      <c r="B48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="16">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="25">
-        <v>4</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="F48" s="24">
+        <v>2.6779999999999999</v>
+      </c>
+      <c r="G48" t="s">
         <v>94</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="H45" t="s">
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="17">
+        <v>6</v>
+      </c>
+      <c r="F49" s="29"/>
+    </row>
+    <row r="50" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="24"/>
-      <c r="B46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="25">
-        <v>4</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="B50" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G46" t="s">
+      <c r="C50" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="H46" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="26" t="s">
+      <c r="D50" s="11">
+        <v>1</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="11">
-        <v>1</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="F48" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>105</v>
-      </c>
-      <c r="B49" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49">
-        <v>4</v>
-      </c>
-      <c r="E49" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B50" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50">
-        <v>4</v>
+      <c r="F50" s="24">
+        <v>0.51</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" s="29"/>
+        <v>100</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="F51" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="25">
-        <v>2</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="G52" t="s">
-        <v>115</v>
-      </c>
-      <c r="H52" t="s">
-        <v>116</v>
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52">
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="13"/>
+        <v>104</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>164</v>
+      </c>
       <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="27"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="16">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>119</v>
-      </c>
-      <c r="B54" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D54">
-        <v>2</v>
+      <c r="E54" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F54" s="24">
+        <v>7.5</v>
+      </c>
+      <c r="G54" t="s">
+        <v>109</v>
+      </c>
+      <c r="H54" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>121</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="D55">
         <v>2</v>
       </c>
-      <c r="F55" s="25"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C56" s="13"/>
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>77</v>
+      </c>
       <c r="D56">
         <v>2</v>
       </c>
-      <c r="E56" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>126</v>
-      </c>
-      <c r="B57" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="C57" s="13"/>
+        <v>115</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>164</v>
+      </c>
       <c r="D57">
         <v>2</v>
       </c>
+      <c r="F57" s="30"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>128</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>129</v>
+      <c r="A58" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="D58">
         <v>2</v>
       </c>
+      <c r="E58" t="s">
+        <v>119</v>
+      </c>
+      <c r="F58" s="24">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>130</v>
-      </c>
-      <c r="B59" s="2"/>
+        <v>120</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="D59">
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B60" s="30"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="25" t="s">
-        <v>78</v>
+      <c r="A60" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>132</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C61" s="13"/>
+        <v>124</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="22" t="s">
+        <v>164</v>
+      </c>
       <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61" t="s">
-        <v>134</v>
-      </c>
-      <c r="G61" t="s">
-        <v>43</v>
-      </c>
-      <c r="H61" t="s">
-        <v>116</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>135</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
+      <c r="A62" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" s="43"/>
+      <c r="C62" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>137</v>
-      </c>
-      <c r="B63" s="28" t="s">
-        <v>138</v>
+        <v>126</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="44" t="s">
+        <v>181</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
+      <c r="E63" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" s="24">
+        <v>5.0720000000000001</v>
+      </c>
       <c r="G63" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="H63" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>141</v>
-      </c>
-      <c r="B64" s="2"/>
+        <v>129</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>164</v>
+      </c>
       <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="G65" t="s">
+        <v>133</v>
+      </c>
+      <c r="H65" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>135</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D66">
         <v>4</v>
       </c>
-      <c r="F64" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C66" s="13"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>144</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D67">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="13"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="D69">
         <f>4+2+1+1+6</f>
         <v>14</v>
       </c>
-      <c r="E67" t="s">
-        <v>146</v>
-      </c>
-      <c r="G67" t="s">
-        <v>147</v>
-      </c>
-      <c r="H67" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>46</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D68">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>150</v>
-      </c>
-      <c r="B69" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="D69">
-        <v>3</v>
+      <c r="E69" t="s">
+        <v>139</v>
+      </c>
+      <c r="F69" s="24">
+        <v>4.05</v>
+      </c>
+      <c r="G69" t="s">
+        <v>140</v>
+      </c>
+      <c r="H69" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>152</v>
-      </c>
-      <c r="B70" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>164</v>
+      </c>
       <c r="D70">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>153</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
+      </c>
+      <c r="B71" s="13"/>
+      <c r="C71" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="E71" t="s">
-        <v>155</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>156</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C72" s="13"/>
+        <v>144</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="22" t="s">
+        <v>164</v>
+      </c>
       <c r="D72">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>17</v>
+        <v>146</v>
+      </c>
+      <c r="C73" s="39" t="s">
+        <v>182</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>159</v>
+        <v>147</v>
+      </c>
+      <c r="F73" s="24">
+        <v>2.4750000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>122</v>
+        <v>149</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
     </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>151</v>
+      </c>
+      <c r="F75" s="24">
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>162</v>
-      </c>
-      <c r="B77" s="30"/>
-      <c r="D77">
-        <v>4</v>
+      <c r="A76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>163</v>
-      </c>
-      <c r="B78" s="30"/>
-      <c r="D78">
-        <v>4</v>
+      <c r="A78" s="8" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>164</v>
-      </c>
-      <c r="B79" s="30"/>
+        <v>154</v>
+      </c>
+      <c r="B79" s="43"/>
+      <c r="C79" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D79">
         <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>165</v>
-      </c>
-      <c r="B80" s="30"/>
+        <v>155</v>
+      </c>
+      <c r="B80" s="43"/>
+      <c r="C80" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D80">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>166</v>
-      </c>
-      <c r="B81" s="30"/>
+        <v>156</v>
+      </c>
+      <c r="B81" s="43"/>
+      <c r="C81" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="D81">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>167</v>
-      </c>
-      <c r="B82" s="30"/>
+        <v>157</v>
+      </c>
+      <c r="B82" s="43"/>
+      <c r="C82" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D82">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>168</v>
-      </c>
-      <c r="B83" s="30"/>
-      <c r="D83" s="25" t="s">
-        <v>78</v>
+        <v>158</v>
+      </c>
+      <c r="B83" s="43"/>
+      <c r="C83" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>159</v>
+      </c>
+      <c r="B84" s="43"/>
+      <c r="C84" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>160</v>
+      </c>
+      <c r="B85" s="43"/>
+      <c r="C85" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D85" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="B39" r:id="rId1"/>
-    <hyperlink ref="E39" r:id="rId2"/>
-    <hyperlink ref="B40" r:id="rId3"/>
-    <hyperlink ref="E40" r:id="rId4"/>
-    <hyperlink ref="E42" r:id="rId5"/>
-    <hyperlink ref="E48" r:id="rId6"/>
+    <hyperlink ref="B41" r:id="rId1"/>
+    <hyperlink ref="B42" r:id="rId2"/>
+    <hyperlink ref="E50" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <ignoredErrors>
+    <ignoredError sqref="C22:C23 C18:C21 C28:C30 C34:C40 C53 C57 C61 C64 C66 C70:C72 C74 C76" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added symbols for all components
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -705,8 +705,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -824,7 +825,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -846,6 +847,7 @@
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1280,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1859,7 +1861,7 @@
       <c r="A40" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C40" s="43" t="s">
@@ -2591,7 +2593,6 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="B39" r:id="rId1"/>
-    <hyperlink ref="B40" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
added all components in Eagle
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="225"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19380" windowHeight="17540" tabRatio="225"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -234,21 +234,12 @@
     <t>?</t>
   </si>
   <si>
-    <t>MIC5209-4.2YS, 4.2V, 500mA</t>
-  </si>
-  <si>
     <t>SOT-223</t>
   </si>
   <si>
     <t>576-2372-ND</t>
   </si>
   <si>
-    <t>AP7333-33SAG-7, 3.3V, 300mA</t>
-  </si>
-  <si>
-    <t>SOT-23-3</t>
-  </si>
-  <si>
     <t>AP7333-33SAG-7DICT-ND</t>
   </si>
   <si>
@@ -279,9 +270,6 @@
     <t>74CBTLV3125PW</t>
   </si>
   <si>
-    <t>14-TSSOP</t>
-  </si>
-  <si>
     <t>568-5262-1-ND</t>
   </si>
   <si>
@@ -495,9 +483,6 @@
     <t>Footprint missing</t>
   </si>
   <si>
-    <t>10-TFSOP</t>
-  </si>
-  <si>
     <t>indv.</t>
   </si>
   <si>
@@ -583,6 +568,21 @@
   </si>
   <si>
     <t>R_ss_prot</t>
+  </si>
+  <si>
+    <t>TSSOP-14</t>
+  </si>
+  <si>
+    <t>TFSOP-10</t>
+  </si>
+  <si>
+    <t>SOT23-3</t>
+  </si>
+  <si>
+    <t>AP7333, 3.3V, 300mA</t>
+  </si>
+  <si>
+    <t>MIC5209, 4.2V, 500mA</t>
   </si>
 </sst>
 </file>
@@ -730,7 +730,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -793,12 +793,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -809,9 +803,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1282,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,7 +1331,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>7</v>
@@ -1422,10 +1413,10 @@
         <v>21</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1436,7 +1427,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
@@ -1456,7 +1447,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
@@ -1477,7 +1468,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D11" s="11">
         <v>2</v>
@@ -1527,7 +1518,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1542,13 +1533,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1567,7 +1558,7 @@
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1585,7 +1576,7 @@
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1593,36 +1584,36 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>175</v>
+        <v>169</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F19" s="22">
         <v>1.78</v>
       </c>
       <c r="G19" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1630,13 +1621,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1644,7 +1635,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1666,13 +1657,13 @@
         <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F25" s="22">
         <v>3.504</v>
@@ -1680,13 +1671,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1694,13 +1685,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1708,10 +1699,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1727,10 +1718,10 @@
         <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1750,7 +1741,7 @@
         <v>52</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1764,7 +1755,7 @@
         <v>54</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1775,7 +1766,7 @@
         <v>55</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1789,7 +1780,7 @@
         <v>57</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1803,7 +1794,7 @@
         <v>59</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1817,7 +1808,7 @@
         <v>61</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1828,7 +1819,7 @@
         <v>62</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1841,10 +1832,10 @@
       <c r="A39" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="28" t="s">
         <v>66</v>
       </c>
       <c r="D39">
@@ -1858,112 +1849,112 @@
       </c>
     </row>
     <row r="40" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="42" t="s">
-        <v>153</v>
-      </c>
-      <c r="B40" s="44" t="s">
+      <c r="A40" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="43" t="s">
+      <c r="D40" s="39">
+        <v>1</v>
+      </c>
+      <c r="E40" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="42">
-        <v>1</v>
-      </c>
-      <c r="E40" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" s="45">
+      <c r="F40" s="42">
         <v>1.19</v>
       </c>
-      <c r="G40" s="41" t="s">
-        <v>159</v>
+      <c r="G40" s="38" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="43" t="s">
+      <c r="C41" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="42" t="s">
+      <c r="D41" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E41" s="43" t="s">
+      <c r="E41" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="45" t="s">
+      <c r="F41" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="G41" s="42" t="s">
-        <v>160</v>
+      <c r="G41" s="39" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="34" t="s">
-        <v>73</v>
+        <v>184</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>183</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F42" s="26">
         <v>0.34800000000000003</v>
       </c>
       <c r="G42" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>181</v>
       </c>
       <c r="D45" s="11">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F45" s="22">
         <v>0.51</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D46" s="11">
         <v>4</v>
@@ -1973,19 +1964,19 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="40" t="s">
-        <v>156</v>
+        <v>108</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F47" s="22">
         <v>5.0720000000000001</v>
@@ -1994,18 +1985,18 @@
         <v>38</v>
       </c>
       <c r="H47" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -2019,7 +2010,7 @@
     </row>
     <row r="50" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B50" s="14"/>
       <c r="C50" s="28"/>
@@ -2028,10 +2019,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>16</v>
@@ -2040,24 +2031,24 @@
         <v>4</v>
       </c>
       <c r="E51" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F51" s="22">
         <v>9.9499999999999993</v>
       </c>
       <c r="G51" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H51" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>16</v>
@@ -2066,24 +2057,24 @@
         <v>4</v>
       </c>
       <c r="E52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F52" s="22">
         <v>2.6779999999999999</v>
       </c>
       <c r="G52" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H52" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>16</v>
@@ -2094,12 +2085,12 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C54" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="34" t="s">
         <v>68</v>
       </c>
       <c r="D54">
@@ -2108,13 +2099,13 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -2128,7 +2119,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="20"/>
@@ -2136,10 +2127,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>16</v>
@@ -2154,18 +2145,18 @@
         <v>7.5</v>
       </c>
       <c r="G58" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H58" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>16</v>
@@ -2176,12 +2167,12 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="34" t="s">
         <v>68</v>
       </c>
       <c r="D60">
@@ -2190,13 +2181,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -2210,7 +2201,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="20"/>
@@ -2218,10 +2209,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>16</v>
@@ -2230,7 +2221,7 @@
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F64" s="22">
         <v>0.74</v>
@@ -2238,10 +2229,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>16</v>
@@ -2252,12 +2243,12 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C66" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="34" t="s">
         <v>68</v>
       </c>
       <c r="D66">
@@ -2266,11 +2257,11 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -2282,14 +2273,14 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B70" s="39"/>
+        <v>166</v>
+      </c>
+      <c r="B70" s="37"/>
       <c r="C70" s="13" t="s">
         <v>16</v>
       </c>
@@ -2299,9 +2290,9 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>172</v>
-      </c>
-      <c r="B71" s="39"/>
+        <v>167</v>
+      </c>
+      <c r="B71" s="37"/>
       <c r="C71" s="13" t="s">
         <v>16</v>
       </c>
@@ -2311,10 +2302,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>110</v>
-      </c>
-      <c r="B72" s="39"/>
-      <c r="C72" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="37"/>
+      <c r="C72" s="35" t="s">
         <v>68</v>
       </c>
       <c r="D72" s="16" t="s">
@@ -2329,33 +2320,33 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C75" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C75" s="34" t="s">
         <v>68</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D76">
         <v>4</v>
@@ -2363,19 +2354,19 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C78" s="13"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C79" s="35" t="s">
-        <v>157</v>
+        <v>118</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="D79">
         <f>4+2+1+1+6</f>
@@ -2388,21 +2379,21 @@
         <v>4.5</v>
       </c>
       <c r="G79" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H79" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>39</v>
       </c>
-      <c r="B80" s="46" t="s">
-        <v>125</v>
+      <c r="B80" s="43" t="s">
+        <v>121</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D80">
         <v>14</v>
@@ -2410,11 +2401,11 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B81" s="13"/>
       <c r="C81" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -2422,11 +2413,11 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D82">
         <v>3</v>
@@ -2434,19 +2425,19 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C83" s="35" t="s">
-        <v>157</v>
+        <v>125</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F83" s="22">
         <v>2.4750000000000001</v>
@@ -2454,13 +2445,13 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2468,19 +2459,19 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C85" s="35" t="s">
-        <v>157</v>
+      <c r="C85" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="D85">
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F85" s="22">
         <v>0.49399999999999999</v>
@@ -2488,13 +2479,13 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -2502,14 +2493,14 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>137</v>
-      </c>
-      <c r="B89" s="39"/>
+        <v>133</v>
+      </c>
+      <c r="B89" s="37"/>
       <c r="C89" s="2" t="s">
         <v>16</v>
       </c>
@@ -2519,9 +2510,9 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>138</v>
-      </c>
-      <c r="B90" s="39"/>
+        <v>134</v>
+      </c>
+      <c r="B90" s="37"/>
       <c r="C90" s="2" t="s">
         <v>16</v>
       </c>
@@ -2531,10 +2522,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>139</v>
-      </c>
-      <c r="B91" s="39"/>
-      <c r="C91" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B91" s="37"/>
+      <c r="C91" s="36" t="s">
         <v>68</v>
       </c>
       <c r="D91">
@@ -2543,9 +2534,9 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>140</v>
-      </c>
-      <c r="B92" s="39"/>
+        <v>136</v>
+      </c>
+      <c r="B92" s="37"/>
       <c r="C92" s="2" t="s">
         <v>16</v>
       </c>
@@ -2555,9 +2546,9 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>141</v>
-      </c>
-      <c r="B93" s="39"/>
+        <v>137</v>
+      </c>
+      <c r="B93" s="37"/>
       <c r="C93" s="2" t="s">
         <v>16</v>
       </c>
@@ -2567,10 +2558,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>142</v>
-      </c>
-      <c r="B94" s="39"/>
-      <c r="C94" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B94" s="37"/>
+      <c r="C94" s="36" t="s">
         <v>68</v>
       </c>
       <c r="D94">
@@ -2579,10 +2570,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>143</v>
-      </c>
-      <c r="B95" s="39"/>
-      <c r="C95" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="B95" s="37"/>
+      <c r="C95" s="36" t="s">
         <v>68</v>
       </c>
       <c r="D95" s="16" t="s">
@@ -2591,9 +2582,6 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <hyperlinks>
-    <hyperlink ref="B39" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
schematic for power domains done
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19380" windowHeight="17540" tabRatio="225"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="225"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="185">
   <si>
     <t>CPIO - Cuisine Purpose Input/Output Board</t>
   </si>
@@ -168,9 +168,6 @@
     <t>VNQ5E160K-E</t>
   </si>
   <si>
-    <t>...</t>
-  </si>
-  <si>
     <t>Power Internal</t>
   </si>
   <si>
@@ -201,18 +198,6 @@
     <t>2.2u</t>
   </si>
   <si>
-    <t>R_sd_1</t>
-  </si>
-  <si>
-    <t>49.9k</t>
-  </si>
-  <si>
-    <t>R_sd_2</t>
-  </si>
-  <si>
-    <t>9.53k</t>
-  </si>
-  <si>
     <t>R_sd_en</t>
   </si>
   <si>
@@ -234,12 +219,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>SOT-223</t>
-  </si>
-  <si>
-    <t>576-2372-ND</t>
-  </si>
-  <si>
     <t>AP7333-33SAG-7DICT-ND</t>
   </si>
   <si>
@@ -474,9 +453,6 @@
     <t>497-11721-1-ND</t>
   </si>
   <si>
-    <t>LDO LED  (5 to 4V)</t>
-  </si>
-  <si>
     <t>Blue</t>
   </si>
   <si>
@@ -489,12 +465,6 @@
     <t>LDO Sensor/ADC (5 to 3.3V)</t>
   </si>
   <si>
-    <t>What is the maximum current for 14 prog. RGB LEDs?</t>
-  </si>
-  <si>
-    <t>Level Shifter (3.3 to 5V) for LED command instead of additional LDO for LEDs. Drive LEDs with 5V</t>
-  </si>
-  <si>
     <t>AOZ1280CI, 1.2 A</t>
   </si>
   <si>
@@ -582,7 +552,34 @@
     <t>AP7333, 3.3V, 300mA</t>
   </si>
   <si>
-    <t>MIC5209, 4.2V, 500mA</t>
+    <t>10M</t>
+  </si>
+  <si>
+    <t>R_sd_1a</t>
+  </si>
+  <si>
+    <t>R_sd_2a</t>
+  </si>
+  <si>
+    <t>R_sd_1b</t>
+  </si>
+  <si>
+    <t>R_sd_2b</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>9.1k</t>
+  </si>
+  <si>
+    <t>C_ldo3.3</t>
+  </si>
+  <si>
+    <t>1u</t>
   </si>
 </sst>
 </file>
@@ -592,7 +589,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -636,6 +633,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -705,7 +709,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -729,8 +733,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -805,18 +823,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -839,6 +850,20 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1271,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J95"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1331,7 +1356,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>7</v>
@@ -1413,10 +1438,10 @@
         <v>21</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1427,7 +1452,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
@@ -1447,7 +1472,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
@@ -1468,7 +1493,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D11" s="11">
         <v>2</v>
@@ -1518,7 +1543,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1533,13 +1558,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1558,7 +1583,7 @@
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="21" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1576,7 +1601,7 @@
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="21" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1584,36 +1609,36 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F19" s="22">
         <v>1.78</v>
       </c>
       <c r="G19" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1621,13 +1646,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>174</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>128</v>
+        <v>164</v>
+      </c>
+      <c r="B21" s="1">
+        <v>100</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1635,7 +1660,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1657,13 +1682,13 @@
         <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F25" s="22">
         <v>3.504</v>
@@ -1671,13 +1696,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1685,13 +1710,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1699,10 +1724,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1710,24 +1735,24 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
         <v>49</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>50</v>
       </c>
       <c r="F31" s="22">
         <v>0.7</v>
@@ -1735,13 +1760,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="C32" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1749,13 +1774,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="C33" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1763,10 +1788,11 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>55</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B34" s="38"/>
       <c r="C34" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1774,13 +1800,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C35" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1788,13 +1814,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>176</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>59</v>
+        <v>180</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1802,13 +1828,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>178</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1816,239 +1842,213 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>177</v>
+      </c>
+      <c r="B38" s="1">
+        <v>430</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D38">
         <v>1</v>
-      </c>
-      <c r="G38" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="28" t="s">
-        <v>66</v>
+        <v>179</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>136</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="E39" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="26">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="26">
         <v>0.311</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="B40" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="39">
-        <v>1</v>
-      </c>
-      <c r="E40" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="F40" s="42">
-        <v>1.19</v>
-      </c>
-      <c r="G40" s="38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="E41" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="G41" s="39" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F42" s="26">
         <v>0.34800000000000003</v>
       </c>
       <c r="G42" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C45" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="D45" s="11">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>81</v>
-      </c>
-      <c r="F45" s="22">
-        <v>0.51</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>157</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>183</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="F43" s="26"/>
+    </row>
+    <row r="44" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>143</v>
+        <v>73</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>171</v>
       </c>
       <c r="D46" s="11">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" s="22">
+        <v>0.51</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="11">
         <v>4</v>
       </c>
-      <c r="E46"/>
-      <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>107</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" s="22">
-        <v>5.0720000000000001</v>
-      </c>
-      <c r="G47" t="s">
-        <v>38</v>
-      </c>
-      <c r="H47" t="s">
-        <v>91</v>
-      </c>
+      <c r="E47"/>
+      <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>143</v>
+        <v>101</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>172</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="14"/>
-      <c r="C49" s="28"/>
-      <c r="E49"/>
-      <c r="F49" s="22"/>
+      <c r="E48" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" s="22">
+        <v>5.0720000000000001</v>
+      </c>
+      <c r="G48" t="s">
+        <v>38</v>
+      </c>
+      <c r="H48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
-        <v>159</v>
-      </c>
       <c r="B50" s="14"/>
       <c r="C50" s="28"/>
       <c r="E50"/>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="16">
-        <v>4</v>
-      </c>
-      <c r="E51" t="s">
-        <v>76</v>
-      </c>
-      <c r="F51" s="22">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="G51" t="s">
-        <v>79</v>
-      </c>
-      <c r="H51" t="s">
-        <v>77</v>
-      </c>
+    <row r="51" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="28"/>
+      <c r="E51"/>
+      <c r="F51" s="22"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>16</v>
@@ -2057,41 +2057,53 @@
         <v>4</v>
       </c>
       <c r="E52" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F52" s="22">
-        <v>2.6779999999999999</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="G52" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="H52" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>83</v>
+      <c r="A53" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="16">
         <v>4</v>
+      </c>
+      <c r="E53" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" s="22">
+        <v>2.6779999999999999</v>
+      </c>
+      <c r="G53" t="s">
+        <v>72</v>
+      </c>
+      <c r="H53" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C54" s="34" t="s">
-        <v>68</v>
+        <v>76</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D54">
         <v>4</v>
@@ -2099,81 +2111,81 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>86</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>143</v>
+        <v>77</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>63</v>
       </c>
       <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="F55" s="25"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="2"/>
-      <c r="C56" s="20"/>
+      <c r="A56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
       <c r="F56" s="25"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="15" t="s">
-        <v>160</v>
-      </c>
       <c r="B57" s="2"/>
       <c r="C57" s="20"/>
       <c r="F57" s="25"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58" s="16">
-        <v>2</v>
-      </c>
-      <c r="E58" s="19">
-        <v>2635</v>
-      </c>
-      <c r="F58" s="22">
-        <v>7.5</v>
-      </c>
-      <c r="G58" t="s">
-        <v>90</v>
-      </c>
-      <c r="H58" t="s">
-        <v>91</v>
-      </c>
+      <c r="A58" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="20"/>
+      <c r="F58" s="25"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>92</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>93</v>
+      <c r="A59" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="16">
         <v>2</v>
+      </c>
+      <c r="E59" s="19">
+        <v>2635</v>
+      </c>
+      <c r="F59" s="22">
+        <v>7.5</v>
+      </c>
+      <c r="G59" t="s">
+        <v>83</v>
+      </c>
+      <c r="H59" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C60" s="34" t="s">
-        <v>68</v>
+        <v>86</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -2181,58 +2193,52 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>96</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="20" t="s">
-        <v>143</v>
+        <v>87</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="34" t="s">
+        <v>63</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
-      <c r="F61" s="27"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="2"/>
-      <c r="C62" s="20"/>
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
       <c r="F62" s="27"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="15" t="s">
-        <v>161</v>
-      </c>
       <c r="B63" s="2"/>
       <c r="C63" s="20"/>
       <c r="F63" s="27"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D64">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s">
-        <v>100</v>
-      </c>
-      <c r="F64" s="22">
-        <v>0.74</v>
-      </c>
+      <c r="A64" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="20"/>
+      <c r="F64" s="27"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>101</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>102</v>
+      <c r="A65" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>16</v>
@@ -2240,16 +2246,22 @@
       <c r="D65">
         <v>2</v>
       </c>
+      <c r="E65" t="s">
+        <v>93</v>
+      </c>
+      <c r="F65" s="22">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C66" s="34" t="s">
-        <v>68</v>
+        <v>95</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -2257,167 +2269,169 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>105</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="20" t="s">
-        <v>143</v>
+        <v>96</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>63</v>
       </c>
       <c r="D67">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>98</v>
+      </c>
       <c r="B68" s="2"/>
-      <c r="C68" s="20"/>
+      <c r="C68" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="15" t="s">
-        <v>163</v>
-      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="20"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B70" s="37"/>
-      <c r="C70" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70" s="16" t="s">
-        <v>68</v>
+      <c r="A70" s="15" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>167</v>
+      <c r="A71" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="B71" s="37"/>
       <c r="C71" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
       <c r="B72" s="37"/>
-      <c r="C72" s="35" t="s">
-        <v>68</v>
+      <c r="C72" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="11"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="19"/>
+      <c r="A73" t="s">
+        <v>99</v>
+      </c>
+      <c r="B73" s="37"/>
+      <c r="C73" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D73" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="15" t="s">
-        <v>164</v>
-      </c>
+      <c r="A74" s="11"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="19"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>112</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C75" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D75">
-        <v>1</v>
-      </c>
-      <c r="H75" t="s">
-        <v>114</v>
+      <c r="A75" s="15" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>115</v>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="20" t="s">
-        <v>143</v>
+        <v>105</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" s="34" t="s">
+        <v>63</v>
       </c>
       <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="H76" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>108</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D77">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C78" s="13"/>
-    </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>117</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D79">
+      <c r="A79" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C79" s="13"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>110</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D80">
         <f>4+2+1+1+6</f>
         <v>14</v>
       </c>
-      <c r="E79">
+      <c r="E80">
         <v>1655</v>
       </c>
-      <c r="F79" s="22">
+      <c r="F80" s="22">
         <v>4.5</v>
       </c>
-      <c r="G79" t="s">
-        <v>119</v>
-      </c>
-      <c r="H79" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>39</v>
-      </c>
-      <c r="B80" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="D80">
-        <v>14</v>
+      <c r="G80" t="s">
+        <v>112</v>
+      </c>
+      <c r="H80" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>122</v>
-      </c>
-      <c r="B81" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="B81" s="38" t="s">
+        <v>114</v>
+      </c>
       <c r="C81" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>123</v>
-      </c>
-      <c r="B82" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="B82" s="13"/>
       <c r="C82" s="20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D82">
         <v>3</v>
@@ -2425,92 +2439,92 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>124</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>152</v>
+        <v>116</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="20" t="s">
+        <v>136</v>
       </c>
       <c r="D83">
-        <v>1</v>
-      </c>
-      <c r="E83" t="s">
-        <v>126</v>
-      </c>
-      <c r="F83" s="22">
-        <v>2.4750000000000001</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C84" s="20" t="s">
-        <v>143</v>
+        <v>118</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D84">
         <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>119</v>
+      </c>
+      <c r="F84" s="22">
+        <v>2.4750000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>152</v>
+        <v>121</v>
+      </c>
+      <c r="C85" s="20" t="s">
+        <v>136</v>
       </c>
       <c r="D85">
         <v>1</v>
-      </c>
-      <c r="E85" t="s">
-        <v>130</v>
-      </c>
-      <c r="F85" s="22">
-        <v>0.49399999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C86" s="20" t="s">
-        <v>143</v>
+        <v>16</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="8" t="s">
-        <v>132</v>
+      <c r="E86" t="s">
+        <v>123</v>
+      </c>
+      <c r="F86" s="22">
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>124</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>133</v>
-      </c>
-      <c r="B89" s="37"/>
-      <c r="C89" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D89">
-        <v>4</v>
+      <c r="A89" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B90" s="37"/>
       <c r="C90" s="2" t="s">
@@ -2522,11 +2536,11 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B91" s="37"/>
-      <c r="C91" s="36" t="s">
-        <v>68</v>
+      <c r="C91" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D91">
         <v>4</v>
@@ -2534,19 +2548,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B92" s="37"/>
-      <c r="C92" s="2" t="s">
-        <v>16</v>
+      <c r="C92" s="36" t="s">
+        <v>63</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B93" s="37"/>
       <c r="C93" s="2" t="s">
@@ -2558,11 +2572,11 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B94" s="37"/>
-      <c r="C94" s="36" t="s">
-        <v>68</v>
+      <c r="C94" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -2570,14 +2584,26 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B95" s="37"/>
       <c r="C95" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D95" s="16" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>132</v>
+      </c>
+      <c r="B96" s="37"/>
+      <c r="C96" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2585,7 +2611,7 @@
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="C26:C28 C32:C38 C55 C61 C67 C76 C80:C82 C84 C86 C48 C17:C18 C20:C21 C46" numberStoredAsText="1"/>
+    <ignoredError sqref="C26:C28 C39:C40 C56 C62 C68 C77 C81:C83 C85 C87 C49 C17:C18 C20:C21 C47 C32:C37 C38 C43" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Level Shifter to Components
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -585,16 +585,16 @@
     <t>Level Shifter for LED command</t>
   </si>
   <si>
-    <t>74LVC1T45GW</t>
-  </si>
-  <si>
-    <t>6-TSSOP</t>
-  </si>
-  <si>
     <t>568-5461-1-ND</t>
   </si>
   <si>
     <t>Level Shifter (3.3 to 5V) for LED command instead of additional LDO for LEDs. Drive LEDs with 5V</t>
+  </si>
+  <si>
+    <t>74LVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-363 </t>
   </si>
 </sst>
 </file>
@@ -724,7 +724,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -762,8 +762,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -841,11 +855,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -875,6 +886,13 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
@@ -882,6 +900,13 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1316,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2448,22 +2473,22 @@
         <v>185</v>
       </c>
       <c r="B82" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C82" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="D82" s="11">
+        <v>1</v>
+      </c>
+      <c r="E82" s="14" t="s">
         <v>186</v>
-      </c>
-      <c r="C82" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="D82" s="11">
-        <v>1</v>
-      </c>
-      <c r="E82" s="14" t="s">
-        <v>188</v>
       </c>
       <c r="F82" s="14">
         <v>0.38700000000000001</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated component list with JST connectors
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="199">
   <si>
     <t>CPIO - Cuisine Purpose Input/Output Board</t>
   </si>
@@ -312,9 +312,6 @@
     <t>Brightness Sensor Plug</t>
   </si>
   <si>
-    <t>2x, JST with cable</t>
-  </si>
-  <si>
     <t>Brightness Sensor Socket</t>
   </si>
   <si>
@@ -345,9 +342,6 @@
     <t>SPI Socket</t>
   </si>
   <si>
-    <t>2x3 Header ?</t>
-  </si>
-  <si>
     <t>GPIO 7 - 11</t>
   </si>
   <si>
@@ -595,6 +589,39 @@
   </si>
   <si>
     <t xml:space="preserve">SOT-363 </t>
+  </si>
+  <si>
+    <t>6x, JST</t>
+  </si>
+  <si>
+    <t>455-2247-ND</t>
+  </si>
+  <si>
+    <t>455-2248-ND</t>
+  </si>
+  <si>
+    <t>455-2249-ND</t>
+  </si>
+  <si>
+    <t>455-2271-ND</t>
+  </si>
+  <si>
+    <t>455-2266-ND</t>
+  </si>
+  <si>
+    <t>455-2219-ND</t>
+  </si>
+  <si>
+    <t>455-2267-ND</t>
+  </si>
+  <si>
+    <t>455-1135-1-ND</t>
+  </si>
+  <si>
+    <t>Plug Crimp Connectors</t>
+  </si>
+  <si>
+    <t>for JST</t>
   </si>
 </sst>
 </file>
@@ -659,7 +686,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -692,12 +719,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -724,7 +745,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -776,8 +797,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -813,9 +838,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
@@ -840,10 +862,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -852,11 +874,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -893,6 +915,8 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
@@ -907,6 +931,8 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1339,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1352,7 +1378,7 @@
     <col min="3" max="3" width="12.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="21" customWidth="1"/>
     <col min="7" max="7" width="80.5" customWidth="1"/>
     <col min="9" max="9" width="7.83203125" customWidth="1"/>
     <col min="10" max="10" width="30.5" customWidth="1"/>
@@ -1377,13 +1403,13 @@
       <c r="E2" s="7">
         <v>42353</v>
       </c>
-      <c r="F2" s="23"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="23"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:10" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -1399,9 +1425,9 @@
         <v>6</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F4" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -1414,11 +1440,11 @@
     <row r="5" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
-      <c r="F5" s="25"/>
-      <c r="I5" s="29" t="s">
+      <c r="F5" s="24"/>
+      <c r="I5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="29" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1428,11 +1454,11 @@
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
-      <c r="F6" s="25"/>
-      <c r="I6" s="31" t="s">
+      <c r="F6" s="24"/>
+      <c r="I6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="29" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1452,11 +1478,11 @@
       <c r="E7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="I7" s="32" t="s">
+      <c r="F7" s="24"/>
+      <c r="I7" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="29" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1476,15 +1502,15 @@
       <c r="E8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>143</v>
+      <c r="I8" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1495,7 +1521,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
@@ -1503,7 +1529,7 @@
       <c r="E9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <v>0.63700000000000001</v>
       </c>
     </row>
@@ -1515,7 +1541,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
@@ -1523,10 +1549,10 @@
       <c r="E10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>2.25</v>
       </c>
-      <c r="G10" s="18"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
@@ -1536,7 +1562,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D11" s="11">
         <v>2</v>
@@ -1544,22 +1570,22 @@
       <c r="E11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="24">
         <v>0.34</v>
       </c>
-      <c r="G11" s="18"/>
+      <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="18"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1575,8 +1601,8 @@
       <c r="E14" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="19"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1586,7 +1612,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1594,20 +1620,20 @@
       <c r="E15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="24">
         <v>0.752</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1615,18 +1641,18 @@
       <c r="E16" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="21">
         <v>2.609</v>
       </c>
-      <c r="G16" s="18"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="21" t="s">
-        <v>136</v>
+      <c r="C17" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1634,7 +1660,7 @@
       <c r="E17" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="21">
         <v>0.20699999999999999</v>
       </c>
     </row>
@@ -1643,8 +1669,8 @@
         <v>42</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="21" t="s">
-        <v>136</v>
+      <c r="C18" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1652,36 +1678,36 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>159</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="F19" s="21">
+        <v>1.78</v>
+      </c>
+      <c r="G19" t="s">
         <v>160</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>161</v>
-      </c>
-      <c r="F19" s="22">
-        <v>1.78</v>
-      </c>
-      <c r="G19" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>136</v>
+      <c r="C20" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1689,13 +1715,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B21" s="1">
         <v>100</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>136</v>
+      <c r="C21" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1703,7 +1729,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1725,27 +1751,27 @@
         <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>139</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="22">
+      <c r="F25" s="21">
         <v>3.504</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>136</v>
+      <c r="C26" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1753,13 +1779,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>136</v>
+        <v>119</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1767,10 +1793,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>168</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>136</v>
+        <v>166</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1786,10 +1812,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1797,7 +1823,7 @@
       <c r="E31" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="21">
         <v>0.7</v>
       </c>
     </row>
@@ -1808,8 +1834,8 @@
       <c r="B32" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>136</v>
+      <c r="C32" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1822,8 +1848,8 @@
       <c r="B33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>136</v>
+      <c r="C33" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1833,9 +1859,9 @@
       <c r="A34" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="20" t="s">
-        <v>136</v>
+      <c r="B34" s="36"/>
+      <c r="C34" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1848,8 +1874,8 @@
       <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>136</v>
+      <c r="C35" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1857,13 +1883,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>136</v>
+        <v>178</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1871,13 +1897,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>136</v>
+        <v>179</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1885,13 +1911,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B38" s="1">
         <v>430</v>
       </c>
-      <c r="C38" s="20" t="s">
-        <v>136</v>
+      <c r="C38" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1899,13 +1925,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>136</v>
+        <v>180</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1916,10 +1942,10 @@
         <v>57</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>136</v>
+        <v>173</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1935,7 +1961,7 @@
       <c r="B41" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="27" t="s">
         <v>61</v>
       </c>
       <c r="D41">
@@ -1944,19 +1970,19 @@
       <c r="E41" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="26">
+      <c r="F41" s="25">
         <v>0.311</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>171</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1964,7 +1990,7 @@
       <c r="E42" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="26">
+      <c r="F42" s="25">
         <v>0.34800000000000003</v>
       </c>
       <c r="G42" t="s">
@@ -1973,18 +1999,18 @@
     </row>
     <row r="43" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>136</v>
+        <v>182</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
-      <c r="F43" s="26"/>
+      <c r="F43" s="25"/>
     </row>
     <row r="44" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1994,13 +2020,13 @@
     </row>
     <row r="46" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C46" s="28" t="s">
-        <v>171</v>
+      <c r="C46" s="27" t="s">
+        <v>169</v>
       </c>
       <c r="D46" s="11">
         <v>1</v>
@@ -2008,46 +2034,46 @@
       <c r="E46" t="s">
         <v>74</v>
       </c>
-      <c r="F46" s="22">
+      <c r="F46" s="21">
         <v>0.51</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>136</v>
+        <v>119</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D47" s="11">
         <v>4</v>
       </c>
       <c r="E47"/>
-      <c r="F47" s="22"/>
+      <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
-        <v>102</v>
-      </c>
-      <c r="F48" s="22">
+      <c r="F48" s="21">
         <v>5.0720000000000001</v>
       </c>
       <c r="G48" t="s">
@@ -2059,62 +2085,57 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>136</v>
+      <c r="C49" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="14"/>
-      <c r="C50" s="28"/>
-      <c r="E50"/>
-      <c r="F50" s="22"/>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>197</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50">
+        <f>D56*3+D62*4+D68*2</f>
+        <v>24</v>
+      </c>
+      <c r="E50" t="s">
+        <v>196</v>
+      </c>
+      <c r="F50" s="21">
+        <v>0.59</v>
+      </c>
     </row>
     <row r="51" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
-        <v>149</v>
-      </c>
       <c r="B51" s="14"/>
-      <c r="C51" s="28"/>
+      <c r="C51" s="27"/>
       <c r="E51"/>
-      <c r="F51" s="22"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="16">
-        <v>4</v>
-      </c>
-      <c r="E52" t="s">
-        <v>69</v>
-      </c>
-      <c r="F52" s="22">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="G52" t="s">
-        <v>72</v>
-      </c>
-      <c r="H52" t="s">
-        <v>70</v>
-      </c>
+      <c r="F51" s="21"/>
+    </row>
+    <row r="52" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B52" s="14"/>
+      <c r="C52" s="27"/>
+      <c r="E52"/>
+      <c r="F52" s="21"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>67</v>
+        <v>150</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>68</v>
@@ -2126,10 +2147,10 @@
         <v>4</v>
       </c>
       <c r="E53" t="s">
-        <v>71</v>
-      </c>
-      <c r="F53" s="22">
-        <v>2.6779999999999999</v>
+        <v>69</v>
+      </c>
+      <c r="F53" s="21">
+        <v>9.9499999999999993</v>
       </c>
       <c r="G53" t="s">
         <v>72</v>
@@ -2139,169 +2160,199 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>76</v>
+      <c r="A54" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="16">
         <v>4</v>
+      </c>
+      <c r="E54" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="21">
+        <v>2.6779999999999999</v>
+      </c>
+      <c r="G54" t="s">
+        <v>72</v>
+      </c>
+      <c r="H54" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C55" s="34" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D55">
         <v>4</v>
       </c>
+      <c r="E55" t="s">
+        <v>194</v>
+      </c>
+      <c r="F55" s="21">
+        <v>0.98</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>190</v>
+      </c>
+      <c r="F56" s="21">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C56" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="F56" s="25"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="2"/>
-      <c r="C57" s="20"/>
-      <c r="F57" s="25"/>
+      <c r="C57" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="24"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="15" t="s">
-        <v>150</v>
-      </c>
       <c r="B58" s="2"/>
-      <c r="C58" s="20"/>
-      <c r="F58" s="25"/>
+      <c r="C58" s="19"/>
+      <c r="F58" s="24"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="19"/>
+      <c r="F59" s="24"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D59" s="16">
-        <v>2</v>
-      </c>
-      <c r="E59" s="19">
-        <v>2635</v>
-      </c>
-      <c r="F59" s="22">
-        <v>7.5</v>
-      </c>
-      <c r="G59" t="s">
-        <v>83</v>
-      </c>
-      <c r="H59" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>86</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="16">
         <v>2</v>
+      </c>
+      <c r="E60" s="18">
+        <v>2635</v>
+      </c>
+      <c r="F60" s="21">
+        <v>7.5</v>
+      </c>
+      <c r="G60" t="s">
+        <v>83</v>
+      </c>
+      <c r="H60" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>87</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" s="34" t="s">
-        <v>63</v>
+        <v>85</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
+      <c r="E61" t="s">
+        <v>195</v>
+      </c>
+      <c r="F61" s="21">
+        <v>0.98</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>89</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C62" s="20" t="s">
-        <v>136</v>
+        <v>87</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>142</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
-      <c r="F62" s="27"/>
+      <c r="E62" t="s">
+        <v>191</v>
+      </c>
+      <c r="F62" s="21">
+        <v>1.94</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="2"/>
-      <c r="C63" s="20"/>
-      <c r="F63" s="27"/>
+      <c r="A63" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="F63" s="26"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="15" t="s">
-        <v>151</v>
-      </c>
       <c r="B64" s="2"/>
-      <c r="C64" s="20"/>
-      <c r="F64" s="27"/>
+      <c r="C64" s="19"/>
+      <c r="F64" s="26"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="19"/>
+      <c r="F65" s="26"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D65">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s">
-        <v>93</v>
-      </c>
-      <c r="F65" s="22">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>94</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>95</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>16</v>
@@ -2309,59 +2360,79 @@
       <c r="D66">
         <v>2</v>
       </c>
+      <c r="E66" t="s">
+        <v>93</v>
+      </c>
+      <c r="F66" s="21">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B67" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" s="34" t="s">
-        <v>63</v>
+      <c r="C67" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="D67">
         <v>2</v>
       </c>
+      <c r="E67" t="s">
+        <v>193</v>
+      </c>
+      <c r="F67" s="21">
+        <v>0.88</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>98</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="20" t="s">
-        <v>136</v>
+        <v>95</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="37" t="s">
+        <v>142</v>
       </c>
       <c r="D68">
         <v>2</v>
       </c>
+      <c r="E68" t="s">
+        <v>189</v>
+      </c>
+      <c r="F68" s="21">
+        <v>1.41</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>97</v>
+      </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="20"/>
+      <c r="C69" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="15" t="s">
-        <v>153</v>
-      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="19"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B71" s="37"/>
-      <c r="C71" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D71" s="16" t="s">
-        <v>63</v>
+      <c r="A71" s="15" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>157</v>
-      </c>
-      <c r="B72" s="37"/>
+      <c r="A72" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B72" s="35"/>
       <c r="C72" s="13" t="s">
         <v>16</v>
       </c>
@@ -2371,240 +2442,246 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>99</v>
-      </c>
-      <c r="B73" s="37"/>
-      <c r="C73" s="35" t="s">
-        <v>63</v>
+        <v>155</v>
+      </c>
+      <c r="B73" s="35"/>
+      <c r="C73" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="D73" s="16" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="11"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="19"/>
+      <c r="A74" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" s="35"/>
+      <c r="C74" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D74" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="15" t="s">
-        <v>154</v>
-      </c>
+      <c r="A75" s="11"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="18"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>105</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="C76" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-      <c r="H76" t="s">
-        <v>107</v>
+      <c r="A76" s="15" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C77" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>192</v>
+      </c>
+      <c r="F77" s="21">
+        <v>2.58</v>
+      </c>
+      <c r="H77" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C80" s="13"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>108</v>
       </c>
-      <c r="B77" s="2"/>
-      <c r="C77" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D77">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="8" t="s">
+      <c r="B81" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C79" s="13"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>110</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D80">
+      <c r="C81" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D81">
         <f>4+2+1+1+6</f>
         <v>14</v>
       </c>
-      <c r="E80">
+      <c r="E81">
         <v>1655</v>
       </c>
-      <c r="F80" s="22">
+      <c r="F81" s="21">
         <v>4.5</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G81" t="s">
+        <v>110</v>
+      </c>
+      <c r="H81" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>39</v>
+      </c>
+      <c r="B82" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="H80" t="s">
+      <c r="C82" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D82">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C83" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" s="11">
+        <v>1</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F83" s="14">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>39</v>
-      </c>
-      <c r="B81" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="C81" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D81">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="B82" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="C82" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="D82" s="11">
-        <v>1</v>
-      </c>
-      <c r="E82" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="F82" s="14">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="G82" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>115</v>
-      </c>
-      <c r="B83" s="13"/>
-      <c r="C83" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D83">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>116</v>
-      </c>
-      <c r="B84" s="2"/>
-      <c r="C84" s="20" t="s">
-        <v>136</v>
+      <c r="B84" s="13"/>
+      <c r="C84" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="D84">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>114</v>
+      </c>
+      <c r="B85" s="2"/>
+      <c r="C85" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="F86" s="21">
+        <v>2.4750000000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>118</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="B87" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F85" s="22">
-        <v>2.4750000000000001</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="C87" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>120</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
         <v>121</v>
       </c>
-      <c r="C86" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="F88" s="21">
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>122</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D87">
-        <v>1</v>
-      </c>
-      <c r="E87" t="s">
+      <c r="B89" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F87" s="22">
-        <v>0.49399999999999999</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>124</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C88" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>126</v>
-      </c>
-      <c r="B91" s="37"/>
-      <c r="C91" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D91">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>127</v>
-      </c>
-      <c r="B92" s="37"/>
+      <c r="B92" s="35"/>
       <c r="C92" s="2" t="s">
         <v>16</v>
       </c>
@@ -2612,35 +2689,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>128</v>
-      </c>
-      <c r="B93" s="37"/>
-      <c r="C93" s="36" t="s">
-        <v>63</v>
+        <v>125</v>
+      </c>
+      <c r="B93" s="35"/>
+      <c r="C93" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D93">
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>129</v>
-      </c>
-      <c r="B94" s="37"/>
-      <c r="C94" s="2" t="s">
-        <v>16</v>
+        <v>126</v>
+      </c>
+      <c r="B94" s="35"/>
+      <c r="C94" s="34" t="s">
+        <v>63</v>
       </c>
       <c r="D94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>130</v>
-      </c>
-      <c r="B95" s="37"/>
+        <v>127</v>
+      </c>
+      <c r="B95" s="35"/>
       <c r="C95" s="2" t="s">
         <v>16</v>
       </c>
@@ -2648,13 +2725,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>131</v>
-      </c>
-      <c r="B96" s="37"/>
-      <c r="C96" s="36" t="s">
-        <v>63</v>
+        <v>128</v>
+      </c>
+      <c r="B96" s="35"/>
+      <c r="C96" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -2662,13 +2739,25 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>132</v>
-      </c>
-      <c r="B97" s="37"/>
-      <c r="C97" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B97" s="35"/>
+      <c r="C97" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D97" s="16" t="s">
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>130</v>
+      </c>
+      <c r="B98" s="35"/>
+      <c r="C98" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D98" s="16" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2677,7 +2766,7 @@
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="C26:C28 C56 C62 C68 C77 C83:C84 C86 C88 C49 C17:C18 C20:C21 C47 C32:C40 C43 C81" numberStoredAsText="1"/>
+    <ignoredError sqref="C26:C28 C57 C63 C69 C78 C84:C85 C87 C89 C49 C17:C18 C20:C21 C47 C32:C40 C43 C82" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new XH connector components added
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="204">
   <si>
     <t>CPIO - Cuisine Purpose Input/Output Board</t>
   </si>
@@ -622,6 +622,21 @@
   </si>
   <si>
     <t>0.1u</t>
+  </si>
+  <si>
+    <t>XH-A-3</t>
+  </si>
+  <si>
+    <t>XH-A-4</t>
+  </si>
+  <si>
+    <t>XH-A-2</t>
+  </si>
+  <si>
+    <t>XH-A-6</t>
+  </si>
+  <si>
+    <t>same a for brightness sensor - ok?</t>
   </si>
 </sst>
 </file>
@@ -745,7 +760,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -768,6 +783,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -878,11 +903,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -923,6 +946,11 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
@@ -941,6 +969,11 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1375,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2118,8 +2151,8 @@
         <v>16</v>
       </c>
       <c r="D50">
-        <f>D56*3+D62*4+D68*2</f>
-        <v>24</v>
+        <f>D56*3+D62*4+D68*2+D93*2</f>
+        <v>32</v>
       </c>
       <c r="E50" t="s">
         <v>195</v>
@@ -2153,7 +2186,7 @@
       <c r="C53" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D53" s="16">
+      <c r="D53" s="18">
         <v>4</v>
       </c>
       <c r="E53" t="s">
@@ -2179,7 +2212,7 @@
       <c r="C54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="16">
+      <c r="D54" s="18">
         <v>4</v>
       </c>
       <c r="E54" t="s">
@@ -2222,8 +2255,8 @@
       <c r="B56" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C56" s="37" t="s">
-        <v>141</v>
+      <c r="C56" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="D56">
         <v>4</v>
@@ -2273,7 +2306,7 @@
       <c r="C60" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="16">
+      <c r="D60" s="18">
         <v>2</v>
       </c>
       <c r="E60" s="18">
@@ -2316,8 +2349,8 @@
       <c r="B62" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="37" t="s">
-        <v>141</v>
+      <c r="C62" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -2404,8 +2437,8 @@
       <c r="B68" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C68" s="37" t="s">
-        <v>141</v>
+      <c r="C68" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -2492,8 +2525,8 @@
       <c r="B77" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="C77" s="37" t="s">
-        <v>141</v>
+      <c r="C77" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -2703,25 +2736,45 @@
       <c r="A93" t="s">
         <v>124</v>
       </c>
-      <c r="B93" s="35"/>
-      <c r="C93" s="2" t="s">
+      <c r="B93" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C93" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D93">
         <v>4</v>
+      </c>
+      <c r="E93" t="s">
+        <v>192</v>
+      </c>
+      <c r="F93" s="21">
+        <v>0.88</v>
+      </c>
+      <c r="G93" s="37" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>125</v>
       </c>
-      <c r="B94" s="35"/>
-      <c r="C94" s="34" t="s">
-        <v>63</v>
+      <c r="B94" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="D94">
         <v>4</v>
       </c>
+      <c r="E94" t="s">
+        <v>188</v>
+      </c>
+      <c r="F94" s="21">
+        <v>1.41</v>
+      </c>
+      <c r="G94" s="37"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">

</xml_diff>

<commit_message>
larger PCB schematic updated, onlyUI missing
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="206">
   <si>
     <t>CPIO - Cuisine Purpose Input/Output Board</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Status LED</t>
   </si>
   <si>
-    <t>475-1410-1-ND</t>
-  </si>
-  <si>
     <t>R_led_12V</t>
   </si>
   <si>
@@ -637,6 +634,15 @@
   </si>
   <si>
     <t>same a for brightness sensor - ok?</t>
+  </si>
+  <si>
+    <t>same a for heating plugs - ok?</t>
+  </si>
+  <si>
+    <t>R_led_5V</t>
+  </si>
+  <si>
+    <t>Diode_hss_load</t>
   </si>
 </sst>
 </file>
@@ -760,7 +766,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -830,8 +836,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -904,8 +926,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -951,6 +976,14 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
@@ -974,6 +1007,14 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1406,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J98"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1466,7 +1507,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>7</v>
@@ -1548,10 +1589,10 @@
         <v>21</v>
       </c>
       <c r="I8" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="29" t="s">
         <v>139</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1562,7 +1603,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
@@ -1582,7 +1623,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
@@ -1603,7 +1644,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11" s="11">
         <v>2</v>
@@ -1653,7 +1694,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1668,13 +1709,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1691,27 +1732,21 @@
       <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="21">
-        <v>0.20699999999999999</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="13"/>
+        <v>41</v>
+      </c>
+      <c r="B18" s="38"/>
       <c r="C18" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1719,36 +1754,23 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>157</v>
+        <v>204</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="20" t="s">
+        <v>132</v>
       </c>
       <c r="D19">
         <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>158</v>
-      </c>
-      <c r="F19" s="21">
-        <v>1.78</v>
-      </c>
-      <c r="G19" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>160</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>162</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B20" s="38"/>
       <c r="C20" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1756,1072 +1778,1124 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21" s="1">
-        <v>100</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>133</v>
+        <v>154</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="D21">
         <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21" s="21">
+        <v>1.78</v>
+      </c>
+      <c r="G21" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>159</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>132</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="G22" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="1">
+        <v>100</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="36"/>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>138</v>
-      </c>
-      <c r="F25" s="21">
-        <v>3.504</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>163</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D26">
-        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>133</v>
+        <v>45</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="D27">
         <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" s="21">
+        <v>3.504</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>162</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>47</v>
+      <c r="A30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B30" s="36"/>
+      <c r="C30" s="19"/>
+      <c r="D30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="36"/>
+      <c r="C31" s="19"/>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="F34" s="21">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="36">
+        <v>0</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="1">
+        <v>430</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" s="25">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>63</v>
+      </c>
+      <c r="F45" s="25">
+        <v>0.34800000000000003</v>
+      </c>
+      <c r="G45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="F46" s="25"/>
+    </row>
+    <row r="47" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D49" s="11">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" s="21">
+        <v>0.51</v>
+      </c>
+      <c r="G49" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>49</v>
-      </c>
-      <c r="F31" s="21">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="36">
-        <v>0</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>173</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>175</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>174</v>
-      </c>
-      <c r="B38" s="1">
-        <v>430</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>176</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="G40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="25">
-        <v>0.311</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>142</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
-        <v>64</v>
-      </c>
-      <c r="F42" s="25">
-        <v>0.34800000000000003</v>
-      </c>
-      <c r="G42" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>180</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D43">
+    </row>
+    <row r="50" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="11">
+        <v>4</v>
+      </c>
+      <c r="E50"/>
+      <c r="F50" s="21"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>100</v>
+      </c>
+      <c r="F51" s="21">
+        <v>5.0720000000000001</v>
+      </c>
+      <c r="G51" t="s">
+        <v>38</v>
+      </c>
+      <c r="H51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>195</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53">
+        <f>D59*3+D65*4+D71*2+D96*2</f>
+        <v>30</v>
+      </c>
+      <c r="E53" t="s">
+        <v>194</v>
+      </c>
+      <c r="F53" s="21">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="14"/>
+      <c r="C54" s="27"/>
+      <c r="E54"/>
+      <c r="F54" s="21"/>
+    </row>
+    <row r="55" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="14"/>
+      <c r="C55" s="27"/>
+      <c r="E55"/>
+      <c r="F55" s="21"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="18">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>68</v>
+      </c>
+      <c r="F56" s="21">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="G56" t="s">
+        <v>71</v>
+      </c>
+      <c r="H56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="18">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>70</v>
+      </c>
+      <c r="F57" s="21">
+        <v>2.6779999999999999</v>
+      </c>
+      <c r="G57" t="s">
+        <v>71</v>
+      </c>
+      <c r="H57" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
+        <v>192</v>
+      </c>
+      <c r="F58" s="21">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F59" s="21">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="F60" s="24"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B61" s="2"/>
+      <c r="C61" s="19"/>
+      <c r="F61" s="24"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="19"/>
+      <c r="F62" s="24"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="18">
         <v>2</v>
       </c>
-      <c r="F43" s="25"/>
-    </row>
-    <row r="44" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="D46" s="11">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>74</v>
-      </c>
-      <c r="F46" s="21">
-        <v>0.51</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D47" s="11">
-        <v>4</v>
-      </c>
-      <c r="E47"/>
-      <c r="F47" s="21"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
-        <v>101</v>
-      </c>
-      <c r="F48" s="21">
-        <v>5.0720000000000001</v>
-      </c>
-      <c r="G48" t="s">
-        <v>38</v>
-      </c>
-      <c r="H48" t="s">
+      <c r="E63" s="18">
+        <v>2635</v>
+      </c>
+      <c r="F63" s="21">
+        <v>7.5</v>
+      </c>
+      <c r="G63" t="s">
+        <v>82</v>
+      </c>
+      <c r="H63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>102</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>196</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="C50" s="13" t="s">
+      <c r="B64" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D50">
-        <f>D56*3+D62*4+D68*2+D93*2</f>
-        <v>32</v>
-      </c>
-      <c r="E50" t="s">
-        <v>195</v>
-      </c>
-      <c r="F50" s="21">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="14"/>
-      <c r="C51" s="27"/>
-      <c r="E51"/>
-      <c r="F51" s="21"/>
-    </row>
-    <row r="52" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="27"/>
-      <c r="E52"/>
-      <c r="F52" s="21"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="18">
-        <v>4</v>
-      </c>
-      <c r="E53" t="s">
-        <v>69</v>
-      </c>
-      <c r="F53" s="21">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="G53" t="s">
-        <v>72</v>
-      </c>
-      <c r="H53" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="18">
-        <v>4</v>
-      </c>
-      <c r="E54" t="s">
-        <v>71</v>
-      </c>
-      <c r="F54" s="21">
-        <v>2.6779999999999999</v>
-      </c>
-      <c r="G54" t="s">
-        <v>72</v>
-      </c>
-      <c r="H54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>75</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55">
-        <v>4</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
         <v>193</v>
       </c>
-      <c r="F55" s="21">
+      <c r="F64" s="21">
         <v>0.98</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C56" s="2" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D56">
-        <v>4</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
         <v>189</v>
       </c>
-      <c r="F56" s="21">
-        <v>1.81</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>79</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="F57" s="24"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="2"/>
-      <c r="C58" s="19"/>
-      <c r="F58" s="24"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="19"/>
-      <c r="F59" s="24"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60" s="18">
-        <v>2</v>
-      </c>
-      <c r="E60" s="18">
-        <v>2635</v>
-      </c>
-      <c r="F60" s="21">
-        <v>7.5</v>
-      </c>
-      <c r="G60" t="s">
-        <v>83</v>
-      </c>
-      <c r="H60" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61">
-        <v>2</v>
-      </c>
-      <c r="E61" t="s">
-        <v>194</v>
-      </c>
-      <c r="F61" s="21">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>87</v>
-      </c>
-      <c r="B62" s="13" t="s">
+      <c r="F65" s="21">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D62">
-        <v>2</v>
-      </c>
-      <c r="E62" t="s">
-        <v>190</v>
-      </c>
-      <c r="F62" s="21">
-        <v>1.94</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="B66" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
-      </c>
-      <c r="F63" s="26"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="2"/>
-      <c r="C64" s="19"/>
-      <c r="F64" s="26"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B65" s="2"/>
-      <c r="C65" s="19"/>
-      <c r="F65" s="26"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>16</v>
+      <c r="C66" s="19" t="s">
+        <v>132</v>
       </c>
       <c r="D66">
         <v>2</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" s="26"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B67" s="2"/>
+      <c r="C67" s="19"/>
+      <c r="F67" s="26"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="19"/>
+      <c r="F68" s="26"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>92</v>
+      </c>
+      <c r="F69" s="21">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>93</v>
       </c>
-      <c r="F66" s="21">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B70" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
+        <v>191</v>
+      </c>
+      <c r="F70" s="21">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>94</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B71" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>187</v>
+      </c>
+      <c r="F71" s="21">
+        <v>1.41</v>
+      </c>
+      <c r="G71" s="37" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>96</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="B72" s="2"/>
+      <c r="C72" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B73" s="2"/>
+      <c r="C73" s="19"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" s="35"/>
+      <c r="C75" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D67">
-        <v>2</v>
-      </c>
-      <c r="E67" t="s">
-        <v>192</v>
-      </c>
-      <c r="F67" s="21">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D68">
-        <v>2</v>
-      </c>
-      <c r="E68" t="s">
-        <v>188</v>
-      </c>
-      <c r="F68" s="21">
-        <v>1.41</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>97</v>
-      </c>
-      <c r="B69" s="2"/>
-      <c r="C69" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="2"/>
-      <c r="C70" s="19"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="11" t="s">
+      <c r="D75" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>153</v>
       </c>
-      <c r="B72" s="35"/>
-      <c r="C72" s="13" t="s">
+      <c r="B76" s="35"/>
+      <c r="C76" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D72" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>154</v>
-      </c>
-      <c r="B73" s="35"/>
-      <c r="C73" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D73" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>98</v>
-      </c>
-      <c r="B74" s="35"/>
-      <c r="C74" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D74" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="11"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="18"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="15" t="s">
-        <v>151</v>
+      <c r="D76" s="16" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77" s="35"/>
+      <c r="C77" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="11"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="18"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>190</v>
+      </c>
+      <c r="F80" s="21">
+        <v>2.58</v>
+      </c>
+      <c r="H80" t="s">
         <v>104</v>
       </c>
-      <c r="B77" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-      <c r="E77" t="s">
-        <v>191</v>
-      </c>
-      <c r="F77" s="21">
-        <v>2.58</v>
-      </c>
-      <c r="H77" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>106</v>
-      </c>
-      <c r="B78" s="2"/>
-      <c r="C78" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D78">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C80" s="13"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>105</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C83" s="13"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>107</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D81">
+      <c r="C84" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D84">
         <f>4+2+1+1+6</f>
         <v>14</v>
       </c>
-      <c r="E81">
+      <c r="E84">
         <v>1655</v>
       </c>
-      <c r="F81" s="21">
+      <c r="F84" s="21">
         <v>4.5</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G84" t="s">
+        <v>109</v>
+      </c>
+      <c r="H84" t="s">
         <v>110</v>
-      </c>
-      <c r="H81" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>39</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D82">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="C83" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="D83" s="11">
-        <v>1</v>
-      </c>
-      <c r="E83" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="F83" s="14">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="G83" s="11" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>112</v>
-      </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D84">
-        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>113</v>
-      </c>
-      <c r="B85" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>197</v>
+      </c>
       <c r="C85" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D85">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>114</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D86">
-        <v>1</v>
-      </c>
-      <c r="E86" t="s">
-        <v>116</v>
-      </c>
-      <c r="F86" s="21">
-        <v>2.4750000000000001</v>
+      <c r="A86" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C86" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="D86" s="11">
+        <v>1</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F86" s="14">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>117</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B87" s="13"/>
       <c r="C87" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>119</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>141</v>
+        <v>112</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" s="19" t="s">
+        <v>132</v>
       </c>
       <c r="D88">
-        <v>1</v>
-      </c>
-      <c r="E88" t="s">
-        <v>120</v>
-      </c>
-      <c r="F88" s="21">
-        <v>0.49399999999999999</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>133</v>
+        <v>114</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
+      <c r="E89" t="s">
+        <v>115</v>
+      </c>
+      <c r="F89" s="21">
+        <v>2.4750000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>116</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="8" t="s">
-        <v>122</v>
+      <c r="A91" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91" t="s">
+        <v>119</v>
+      </c>
+      <c r="F91" s="21">
+        <v>0.49399999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>123</v>
-      </c>
-      <c r="B92" s="35"/>
-      <c r="C92" s="2" t="s">
-        <v>16</v>
+        <v>120</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>132</v>
       </c>
       <c r="D92">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>124</v>
-      </c>
-      <c r="B93" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C93" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D93">
-        <v>4</v>
-      </c>
-      <c r="E93" t="s">
-        <v>192</v>
-      </c>
-      <c r="F93" s="21">
-        <v>0.88</v>
-      </c>
-      <c r="G93" s="37" t="s">
-        <v>203</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>125</v>
-      </c>
-      <c r="B94" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D94">
-        <v>4</v>
-      </c>
-      <c r="E94" t="s">
-        <v>188</v>
-      </c>
-      <c r="F94" s="21">
-        <v>1.41</v>
-      </c>
-      <c r="G94" s="37"/>
+      <c r="A94" s="8" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B95" s="35"/>
       <c r="C95" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>123</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96">
+        <v>4</v>
+      </c>
+      <c r="E96" t="s">
+        <v>191</v>
+      </c>
+      <c r="F96" s="21">
+        <v>0.88</v>
+      </c>
+      <c r="G96" s="37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>124</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D97">
+        <v>4</v>
+      </c>
+      <c r="E97" t="s">
+        <v>187</v>
+      </c>
+      <c r="F97" s="21">
+        <v>1.41</v>
+      </c>
+      <c r="G97" s="37"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>125</v>
+      </c>
+      <c r="B98" s="35"/>
+      <c r="C98" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>126</v>
+      </c>
+      <c r="B99" s="35"/>
+      <c r="C99" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>127</v>
       </c>
-      <c r="B96" s="35"/>
-      <c r="C96" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="B100" s="35"/>
+      <c r="C100" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>128</v>
       </c>
-      <c r="B97" s="35"/>
-      <c r="C97" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="D97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>129</v>
-      </c>
-      <c r="B98" s="35"/>
-      <c r="C98" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="D98" s="16" t="s">
-        <v>63</v>
+      <c r="B101" s="35"/>
+      <c r="C101" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2829,7 +2903,7 @@
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="C26:C28 C57 C63 C69 C78 C84:C85 C87 C89 C49 C17:C18 C20:C21 C47 C32:C40 C43 C82" numberStoredAsText="1"/>
+    <ignoredError sqref="C60 C66 C72 C81 C87:C88 C90 C92 C52 C22:C23 C50 C35:C43 C46 C85 C17:C20 C28:C29" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
schematic ready for UX
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -1449,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87:B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2656,7 +2656,7 @@
       <c r="G84" t="s">
         <v>109</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H84" s="37" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2701,7 +2701,7 @@
       <c r="A87" t="s">
         <v>111</v>
       </c>
-      <c r="B87" s="13"/>
+      <c r="B87" s="38"/>
       <c r="C87" s="19" t="s">
         <v>132</v>
       </c>
@@ -2713,7 +2713,7 @@
       <c r="A88" t="s">
         <v>112</v>
       </c>
-      <c r="B88" s="2"/>
+      <c r="B88" s="36"/>
       <c r="C88" s="19" t="s">
         <v>132</v>
       </c>

</xml_diff>

<commit_message>
RGB LEDs added to schematic
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="207">
   <si>
     <t>CPIO - Cuisine Purpose Input/Output Board</t>
   </si>
@@ -643,6 +643,9 @@
   </si>
   <si>
     <t>Diode_hss_load</t>
+  </si>
+  <si>
+    <t>R_rgbled</t>
   </si>
 </sst>
 </file>
@@ -766,7 +769,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -852,8 +855,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -929,8 +934,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -984,6 +992,7 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
@@ -1015,6 +1024,7 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1447,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87:B88"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,8 +1743,8 @@
         <v>40</v>
       </c>
       <c r="B17" s="38"/>
-      <c r="C17" s="20" t="s">
-        <v>132</v>
+      <c r="C17" s="39">
+        <v>1206</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -2220,7 +2230,7 @@
         <v>16</v>
       </c>
       <c r="D53">
-        <f>D59*3+D65*4+D71*2+D96*2</f>
+        <f>D59*3+D65*4+D71*2+D97*2</f>
         <v>30</v>
       </c>
       <c r="E53" t="s">
@@ -2644,8 +2654,7 @@
         <v>140</v>
       </c>
       <c r="D84">
-        <f>4+2+1+1+6</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E84">
         <v>1655</v>
@@ -2671,51 +2680,51 @@
         <v>132</v>
       </c>
       <c r="D85">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="11" t="s">
+      <c r="A86" t="s">
+        <v>206</v>
+      </c>
+      <c r="B86" s="36"/>
+      <c r="C86" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B87" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C86" s="27" t="s">
+      <c r="C87" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="D86" s="11">
-        <v>1</v>
-      </c>
-      <c r="E86" s="14" t="s">
+      <c r="D87" s="11">
+        <v>1</v>
+      </c>
+      <c r="E87" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="F86" s="14">
+      <c r="F87" s="14">
         <v>0.38700000000000001</v>
       </c>
-      <c r="G86" s="11" t="s">
+      <c r="G87" s="11" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>111</v>
-      </c>
-      <c r="B87" s="38"/>
-      <c r="C87" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D87">
-        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>112</v>
-      </c>
-      <c r="B88" s="36"/>
-      <c r="C88" s="19" t="s">
-        <v>132</v>
+        <v>111</v>
+      </c>
+      <c r="B88" s="38"/>
+      <c r="C88" s="19">
+        <v>1206</v>
       </c>
       <c r="D88">
         <v>3</v>
@@ -2723,148 +2732,148 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>113</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>140</v>
+        <v>112</v>
+      </c>
+      <c r="B89" s="36"/>
+      <c r="C89" s="19" t="s">
+        <v>132</v>
       </c>
       <c r="D89">
-        <v>1</v>
-      </c>
-      <c r="E89" t="s">
-        <v>115</v>
-      </c>
-      <c r="F89" s="21">
-        <v>2.4750000000000001</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C90" s="19" t="s">
-        <v>132</v>
+        <v>114</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="D90">
         <v>1</v>
+      </c>
+      <c r="E90" t="s">
+        <v>115</v>
+      </c>
+      <c r="F90" s="21">
+        <v>2.4750000000000001</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>140</v>
+        <v>117</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>132</v>
       </c>
       <c r="D91">
         <v>1</v>
-      </c>
-      <c r="E91" t="s">
-        <v>119</v>
-      </c>
-      <c r="F91" s="21">
-        <v>0.49399999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
+        <v>119</v>
+      </c>
+      <c r="F92" s="21">
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>120</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="19" t="s">
+      <c r="C93" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="D92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="8" t="s">
+      <c r="D93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="8" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>122</v>
-      </c>
-      <c r="B95" s="35"/>
-      <c r="C95" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D95">
-        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>123</v>
-      </c>
-      <c r="B96" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C96" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B96" s="35"/>
+      <c r="C96" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D96">
         <v>4</v>
       </c>
-      <c r="E96" t="s">
-        <v>191</v>
-      </c>
-      <c r="F96" s="21">
-        <v>0.88</v>
-      </c>
-      <c r="G96" s="37" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B97" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>200</v>
+      <c r="C97" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="D97">
         <v>4</v>
       </c>
       <c r="E97" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F97" s="21">
-        <v>1.41</v>
-      </c>
-      <c r="G97" s="37"/>
+        <v>0.88</v>
+      </c>
+      <c r="G97" s="37" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>125</v>
-      </c>
-      <c r="B98" s="35"/>
+        <v>124</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>95</v>
+      </c>
       <c r="C98" s="2" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="D98">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E98" t="s">
+        <v>187</v>
+      </c>
+      <c r="F98" s="21">
+        <v>1.41</v>
+      </c>
+      <c r="G98" s="37"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B99" s="35"/>
       <c r="C99" s="2" t="s">
@@ -2876,11 +2885,11 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B100" s="35"/>
-      <c r="C100" s="34" t="s">
-        <v>62</v>
+      <c r="C100" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -2888,13 +2897,25 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B101" s="35"/>
       <c r="C101" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D101" s="16" t="s">
+      <c r="D101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>128</v>
+      </c>
+      <c r="B102" s="35"/>
+      <c r="C102" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D102" s="16" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2903,7 +2924,7 @@
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="C60 C66 C72 C81 C87:C88 C90 C92 C52 C22:C23 C50 C35:C43 C46 C85 C17:C20 C28:C29" numberStoredAsText="1"/>
+    <ignoredError sqref="C60 C66 C72 C81 C89 C91 C93 C52 C22:C23 C50 C35:C43 C46 C85 C18:C20 C28:C29" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated component list, ordered bom
</commit_message>
<xml_diff>
--- a/cpio-pcb/components/list.xlsx
+++ b/cpio-pcb/components/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="225"/>
+    <workbookView xWindow="0" yWindow="1020" windowWidth="28720" windowHeight="17540" tabRatio="225"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="192">
   <si>
     <t>CPIO - Cuisine Purpose Input/Output Board</t>
   </si>
@@ -120,9 +120,6 @@
     <t>AE10793-ND</t>
   </si>
   <si>
-    <t>Power Input</t>
-  </si>
-  <si>
     <t>Power Supply 12V 2A</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>CP-047A-ND</t>
   </si>
   <si>
-    <t>EG5137-ND</t>
-  </si>
-  <si>
     <t>via I2C</t>
   </si>
   <si>
@@ -150,12 +144,6 @@
     <t>Status LED</t>
   </si>
   <si>
-    <t>R_led_12V</t>
-  </si>
-  <si>
-    <t>diode or switch to put 5V from USB raspi to power output if no supply is connected</t>
-  </si>
-  <si>
     <t>Power Output</t>
   </si>
   <si>
@@ -174,21 +162,9 @@
     <t>785-1277-1-ND</t>
   </si>
   <si>
-    <t>C_sd_1</t>
-  </si>
-  <si>
-    <t>4.7u</t>
-  </si>
-  <si>
-    <t>C_sd_2</t>
-  </si>
-  <si>
     <t>10u</t>
   </si>
   <si>
-    <t>C_sd_3</t>
-  </si>
-  <si>
     <t>L_sd_1</t>
   </si>
   <si>
@@ -330,9 +306,6 @@
     <t>296-38849-1-ND</t>
   </si>
   <si>
-    <t>C_decap_adc</t>
-  </si>
-  <si>
     <t>100n</t>
   </si>
   <si>
@@ -360,33 +333,12 @@
     <t>GPIO 18</t>
   </si>
   <si>
-    <t>Random Status LED</t>
-  </si>
-  <si>
-    <t>R_led_3.3V</t>
-  </si>
-  <si>
-    <t>Beeper</t>
-  </si>
-  <si>
-    <t>AI-1441-TWT-12V-R</t>
-  </si>
-  <si>
-    <t>668-1459-ND</t>
-  </si>
-  <si>
-    <t>R_beeper</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
     <t>Button</t>
   </si>
   <si>
-    <t>EG4791-ND</t>
-  </si>
-  <si>
     <t>R_button</t>
   </si>
   <si>
@@ -420,15 +372,9 @@
     <t>indiv.</t>
   </si>
   <si>
-    <t>500SSP1S2M2, 28V, 5A</t>
-  </si>
-  <si>
     <t>0805</t>
   </si>
   <si>
-    <t>Diode</t>
-  </si>
-  <si>
     <t>2.75mm (diameter)</t>
   </si>
   <si>
@@ -510,21 +456,6 @@
     <t>R_cm_load</t>
   </si>
   <si>
-    <t>1m</t>
-  </si>
-  <si>
-    <t>R_hss_prot</t>
-  </si>
-  <si>
-    <t>R_hss_gnd</t>
-  </si>
-  <si>
-    <t>Diode_hss_gnd</t>
-  </si>
-  <si>
-    <t>Power Slide Switch</t>
-  </si>
-  <si>
     <t>R_ss_prot</t>
   </si>
   <si>
@@ -540,33 +471,6 @@
     <t>AP7333, 3.3V, 300mA</t>
   </si>
   <si>
-    <t>10M</t>
-  </si>
-  <si>
-    <t>R_sd_1a</t>
-  </si>
-  <si>
-    <t>R_sd_2a</t>
-  </si>
-  <si>
-    <t>R_sd_1b</t>
-  </si>
-  <si>
-    <t>R_sd_2b</t>
-  </si>
-  <si>
-    <t>20k</t>
-  </si>
-  <si>
-    <t>30k</t>
-  </si>
-  <si>
-    <t>9.1k</t>
-  </si>
-  <si>
-    <t>C_ldo3.3</t>
-  </si>
-  <si>
     <t>1u</t>
   </si>
   <si>
@@ -639,13 +543,64 @@
     <t>same a for heating plugs - ok?</t>
   </si>
   <si>
-    <t>R_led_5V</t>
-  </si>
-  <si>
-    <t>Diode_hss_load</t>
-  </si>
-  <si>
-    <t>R_rgbled</t>
+    <t>SW400-ND</t>
+  </si>
+  <si>
+    <t>R_sd_2</t>
+  </si>
+  <si>
+    <t>R_sd_1</t>
+  </si>
+  <si>
+    <t>Power Diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>160-1423-1-ND</t>
+  </si>
+  <si>
+    <t>R_led</t>
+  </si>
+  <si>
+    <t>R_cm_u0</t>
+  </si>
+  <si>
+    <t>R_cm_u1</t>
+  </si>
+  <si>
+    <t>Green, V_F=2.1V</t>
+  </si>
+  <si>
+    <t>SBR15A30SP5-13DICT-ND</t>
+  </si>
+  <si>
+    <t>AP02002</t>
+  </si>
+  <si>
+    <t>10m</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C_sd</t>
+  </si>
+  <si>
+    <t>C_ldo</t>
+  </si>
+  <si>
+    <t>15k</t>
+  </si>
+  <si>
+    <t>82k</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
+    <t>10A</t>
   </si>
 </sst>
 </file>
@@ -769,7 +724,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -857,8 +812,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -927,18 +896,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -993,6 +959,13 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
@@ -1025,6 +998,13 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1457,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="99" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1517,7 +1497,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>7</v>
@@ -1599,10 +1579,10 @@
         <v>21</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1613,7 +1593,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
@@ -1633,7 +1613,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
@@ -1654,7 +1634,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D11" s="11">
         <v>2</v>
@@ -1675,13 +1655,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>31</v>
+        <v>176</v>
       </c>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -1691,26 +1671,26 @@
         <v>1</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="24"/>
       <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="F15" s="24">
         <v>0.752</v>
@@ -1719,68 +1699,88 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>130</v>
+        <v>191</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>183</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>182</v>
       </c>
       <c r="F16" s="21">
-        <v>2.609</v>
-      </c>
-      <c r="G16" s="17"/>
+        <v>0.68</v>
+      </c>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39">
-        <v>1206</v>
+        <v>38</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>115</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="20" t="s">
-        <v>132</v>
+        <v>178</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>115</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>204</v>
-      </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="20" t="s">
-        <v>132</v>
+        <v>136</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D19">
         <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="21">
+        <v>1.78</v>
+      </c>
+      <c r="G19" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B20" s="38"/>
+        <v>141</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="C20" s="20" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1788,36 +1788,27 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>156</v>
+        <v>81</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>115</v>
       </c>
       <c r="D21">
         <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>157</v>
-      </c>
-      <c r="F21" s="21">
-        <v>1.78</v>
-      </c>
-      <c r="G21" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>161</v>
+        <v>81</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1825,1098 +1816,932 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="1">
-        <v>100</v>
+        <v>180</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" s="36"/>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="G24" s="37" t="s">
-        <v>42</v>
-      </c>
+      <c r="B24"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="A26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>186</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>137</v>
-      </c>
-      <c r="F27" s="21">
-        <v>3.504</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>163</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G28" s="18"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>205</v>
-      </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="19"/>
-      <c r="D30">
-        <v>1</v>
+      <c r="A30" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>164</v>
-      </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="D31">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>119</v>
+      </c>
+      <c r="F31" s="21">
+        <v>3.504</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F34" s="21">
         <v>0.7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="1" t="s">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B39" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C39" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="36">
-        <v>0</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="F39" s="25">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>172</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>174</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>173</v>
-      </c>
-      <c r="B41" s="1">
-        <v>430</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>175</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="F40" s="25">
+        <v>0.34800000000000003</v>
+      </c>
+      <c r="G40" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="G43" t="s">
+    </row>
+    <row r="41" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="43" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="11">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="21">
+        <v>0.51</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="11">
+        <v>4</v>
+      </c>
+      <c r="E44"/>
+      <c r="F44" s="21"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="21">
+        <v>5.0720000000000001</v>
+      </c>
+      <c r="G45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>163</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46">
+        <f>D52*3+D58*4+D64*2+D86*2</f>
+        <v>30</v>
+      </c>
+      <c r="E46" t="s">
+        <v>162</v>
+      </c>
+      <c r="F46" s="21">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="14"/>
+      <c r="C47" s="27"/>
+      <c r="E47"/>
+      <c r="F47" s="21"/>
+    </row>
+    <row r="48" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="27"/>
+      <c r="E48"/>
+      <c r="F48" s="21"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="18">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="21">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="G49" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B50" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="C50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="18">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" s="21">
+        <v>2.6779999999999999</v>
+      </c>
+      <c r="G50" t="s">
+        <v>63</v>
+      </c>
+      <c r="H50" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="25">
-        <v>0.311</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>141</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="C45" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>63</v>
-      </c>
-      <c r="F45" s="25">
-        <v>0.34800000000000003</v>
-      </c>
-      <c r="G45" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>179</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-      <c r="F46" s="25"/>
-    </row>
-    <row r="47" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="D49" s="11">
-        <v>1</v>
-      </c>
-      <c r="E49" t="s">
-        <v>73</v>
-      </c>
-      <c r="F49" s="21">
-        <v>0.51</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D50" s="11">
-        <v>4</v>
-      </c>
-      <c r="E50"/>
-      <c r="F50" s="21"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>168</v>
+        <v>66</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E51" t="s">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="F51" s="21">
-        <v>5.0720000000000001</v>
-      </c>
-      <c r="G51" t="s">
-        <v>38</v>
-      </c>
-      <c r="H51" t="s">
-        <v>83</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>132</v>
+        <v>68</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>156</v>
+      </c>
+      <c r="F52" s="21">
+        <v>1.81</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>195</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>16</v>
+        <v>70</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="D53">
-        <f>D59*3+D65*4+D71*2+D97*2</f>
-        <v>30</v>
-      </c>
-      <c r="E53" t="s">
-        <v>194</v>
-      </c>
-      <c r="F53" s="21">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="14"/>
-      <c r="C54" s="27"/>
-      <c r="E54"/>
-      <c r="F54" s="21"/>
-    </row>
-    <row r="55" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F53" s="24"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="2"/>
+      <c r="C54" s="19"/>
+      <c r="F54" s="24"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B55" s="14"/>
-      <c r="C55" s="27"/>
-      <c r="E55"/>
-      <c r="F55" s="21"/>
+        <v>128</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="19"/>
+      <c r="F55" s="24"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>148</v>
+        <v>72</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D56" s="18">
-        <v>4</v>
-      </c>
-      <c r="E56" t="s">
-        <v>68</v>
+        <v>2</v>
+      </c>
+      <c r="E56" s="18">
+        <v>2635</v>
       </c>
       <c r="F56" s="21">
-        <v>9.9499999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="G56" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H56" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D57" s="18">
-        <v>4</v>
+      <c r="D57">
+        <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
       <c r="F57" s="21">
-        <v>2.6779999999999999</v>
-      </c>
-      <c r="G57" t="s">
-        <v>71</v>
-      </c>
-      <c r="H57" t="s">
-        <v>69</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>16</v>
+        <v>167</v>
       </c>
       <c r="D58">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="F58" s="21">
-        <v>0.98</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>76</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>198</v>
+        <v>80</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="D59">
-        <v>4</v>
-      </c>
-      <c r="E59" t="s">
-        <v>188</v>
-      </c>
-      <c r="F59" s="21">
-        <v>1.81</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F59" s="26"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>78</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="F60" s="24"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="19"/>
+      <c r="F60" s="26"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
+        <v>129</v>
+      </c>
       <c r="B61" s="2"/>
       <c r="C61" s="19"/>
-      <c r="F61" s="24"/>
+      <c r="F61" s="26"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="19"/>
-      <c r="F62" s="24"/>
+      <c r="A62" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>84</v>
+      </c>
+      <c r="F62" s="21">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>81</v>
+      <c r="A63" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D63" s="18">
-        <v>2</v>
-      </c>
-      <c r="E63" s="18">
-        <v>2635</v>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>159</v>
       </c>
       <c r="F63" s="21">
-        <v>7.5</v>
-      </c>
-      <c r="G63" t="s">
-        <v>82</v>
-      </c>
-      <c r="H63" t="s">
-        <v>83</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>16</v>
+        <v>87</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="F64" s="21">
-        <v>0.98</v>
+        <v>1.41</v>
+      </c>
+      <c r="G64" s="36" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>86</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>199</v>
+        <v>88</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="D65">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s">
-        <v>189</v>
-      </c>
-      <c r="F65" s="21">
-        <v>1.94</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>88</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D66">
-        <v>2</v>
-      </c>
-      <c r="F66" s="26"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="19"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B67" s="2"/>
-      <c r="C67" s="19"/>
-      <c r="F67" s="26"/>
+      <c r="A67" s="15" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="19"/>
-      <c r="F68" s="26"/>
+      <c r="A68" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="35"/>
+      <c r="C68" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="A69" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="35"/>
       <c r="C69" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-      <c r="E69" t="s">
-        <v>92</v>
-      </c>
-      <c r="F69" s="21">
-        <v>0.74</v>
+      <c r="D69" s="16" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>93</v>
-      </c>
-      <c r="B70" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B70" s="35"/>
+      <c r="C70" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="11"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="18"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>94</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>158</v>
+      </c>
+      <c r="F73" s="21">
+        <v>2.58</v>
+      </c>
+      <c r="H73" t="s">
         <v>95</v>
       </c>
-      <c r="C70" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70" t="s">
-        <v>191</v>
-      </c>
-      <c r="F70" s="21">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>94</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="E71" t="s">
-        <v>187</v>
-      </c>
-      <c r="F71" s="21">
-        <v>1.41</v>
-      </c>
-      <c r="G71" s="37" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>96</v>
       </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="2"/>
-      <c r="C73" s="19"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B75" s="35"/>
-      <c r="C75" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75" s="16" t="s">
-        <v>62</v>
+      <c r="B74" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D74">
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>153</v>
-      </c>
-      <c r="B76" s="35"/>
-      <c r="C76" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D76" s="16" t="s">
-        <v>62</v>
-      </c>
+      <c r="A76" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C76" s="13"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>97</v>
-      </c>
-      <c r="B77" s="35"/>
-      <c r="C77" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D77" s="16" t="s">
-        <v>62</v>
+        <v>98</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D77">
+        <v>4</v>
+      </c>
+      <c r="E77">
+        <v>1655</v>
+      </c>
+      <c r="F77" s="21">
+        <v>4.5</v>
+      </c>
+      <c r="G77" t="s">
+        <v>100</v>
+      </c>
+      <c r="H77" s="36" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="11"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="18"/>
+      <c r="A78" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="D79" s="11">
+        <v>1</v>
+      </c>
+      <c r="E79" s="14" t="s">
         <v>150</v>
+      </c>
+      <c r="F79" s="14">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>103</v>
       </c>
-      <c r="B80" s="13" t="s">
-        <v>186</v>
+      <c r="B80" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>201</v>
+        <v>122</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="F80" s="21">
-        <v>2.58</v>
-      </c>
-      <c r="H80" t="s">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="B81" s="1">
+        <v>100</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>104</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C81" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D81">
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" s="35"/>
+      <c r="C85" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C83" s="13"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>107</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B86" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86">
+        <v>4</v>
+      </c>
+      <c r="E86" t="s">
+        <v>159</v>
+      </c>
+      <c r="F86" s="21">
+        <v>0.88</v>
+      </c>
+      <c r="G86" s="36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>108</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D84">
-        <v>12</v>
-      </c>
-      <c r="E84">
-        <v>1655</v>
-      </c>
-      <c r="F84" s="21">
-        <v>4.5</v>
-      </c>
-      <c r="G84" t="s">
+      <c r="B87" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D87">
+        <v>4</v>
+      </c>
+      <c r="E87" t="s">
+        <v>155</v>
+      </c>
+      <c r="F87" s="21">
+        <v>1.41</v>
+      </c>
+      <c r="G87" s="36"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>109</v>
       </c>
-      <c r="H84" s="37" t="s">
+      <c r="B88" s="35"/>
+      <c r="C88" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>39</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D85">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>206</v>
-      </c>
-      <c r="B86" s="36"/>
-      <c r="C86" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="B87" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C87" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="D87" s="11">
-        <v>1</v>
-      </c>
-      <c r="E87" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="F87" s="14">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="G87" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="B89" s="35"/>
+      <c r="C89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>111</v>
       </c>
-      <c r="B88" s="38"/>
-      <c r="C88" s="19">
-        <v>1206</v>
-      </c>
-      <c r="D88">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="B90" s="35"/>
+      <c r="C90" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>112</v>
       </c>
-      <c r="B89" s="36"/>
-      <c r="C89" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D89">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>113</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D90">
-        <v>1</v>
-      </c>
-      <c r="E90" t="s">
-        <v>115</v>
-      </c>
-      <c r="F90" s="21">
-        <v>2.4750000000000001</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>116</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C91" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>118</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D92">
-        <v>1</v>
-      </c>
-      <c r="E92" t="s">
-        <v>119</v>
-      </c>
-      <c r="F92" s="21">
-        <v>0.49399999999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>120</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C93" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>122</v>
-      </c>
-      <c r="B96" s="35"/>
-      <c r="C96" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D96">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>123</v>
-      </c>
-      <c r="B97" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C97" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D97">
-        <v>4</v>
-      </c>
-      <c r="E97" t="s">
-        <v>191</v>
-      </c>
-      <c r="F97" s="21">
-        <v>0.88</v>
-      </c>
-      <c r="G97" s="37" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>124</v>
-      </c>
-      <c r="B98" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D98">
-        <v>4</v>
-      </c>
-      <c r="E98" t="s">
-        <v>187</v>
-      </c>
-      <c r="F98" s="21">
-        <v>1.41</v>
-      </c>
-      <c r="G98" s="37"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>125</v>
-      </c>
-      <c r="B99" s="35"/>
-      <c r="C99" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>126</v>
-      </c>
-      <c r="B100" s="35"/>
-      <c r="C100" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>127</v>
-      </c>
-      <c r="B101" s="35"/>
-      <c r="C101" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>128</v>
-      </c>
-      <c r="B102" s="35"/>
-      <c r="C102" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D102" s="16" t="s">
-        <v>62</v>
+      <c r="B91" s="35"/>
+      <c r="C91" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2924,7 +2749,7 @@
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="C60 C66 C72 C81 C89 C91 C93 C52 C22:C23 C50 C35:C43 C46 C85 C18:C20 C28:C29" numberStoredAsText="1"/>
+    <ignoredError sqref="C53 C59 C65 C74 C81 C20:C23 C44 C35:C36 C78 C37 C38 C17:C18" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>